<commit_message>
Progress on short params
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="597" uniqueCount="274">
   <si>
     <t>Requirement</t>
   </si>
@@ -1010,7 +1010,10 @@
   <autoFilter ref="A1:D178">
     <filterColumn colId="0">
       <filters>
-        <filter val="requirements_class_PrimeMeridianGeoKey"/>
+        <filter val="requirements_class_EllipsoidGeoKey"/>
+        <filter val="requirements_class_EllipsoidInvFlatteningGeoKey"/>
+        <filter val="requirements_class_EllipsoidSemiMajorAxisGeoKey"/>
+        <filter val="requirements_class_EllipsoidSemiMinorAxisGeoKey"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1294,7 +1297,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1379,7 +1382,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>179</v>
       </c>
@@ -1389,9 +1392,11 @@
       <c r="C7" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D7" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>179</v>
       </c>
@@ -1401,9 +1406,11 @@
       <c r="C8" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>179</v>
       </c>
@@ -1413,9 +1420,11 @@
       <c r="C9" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D9" s="2"/>
-    </row>
-    <row r="10" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D9" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>179</v>
       </c>
@@ -1425,9 +1434,11 @@
       <c r="C10" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D10" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>179</v>
       </c>
@@ -1437,9 +1448,11 @@
       <c r="C11" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D11" s="2"/>
-    </row>
-    <row r="12" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D11" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>179</v>
       </c>
@@ -1449,9 +1462,11 @@
       <c r="C12" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D12" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>200</v>
       </c>
@@ -1463,7 +1478,7 @@
       </c>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>200</v>
       </c>
@@ -1475,7 +1490,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>188</v>
       </c>
@@ -1487,7 +1502,7 @@
       </c>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>188</v>
       </c>
@@ -1499,7 +1514,7 @@
       </c>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>188</v>
       </c>
@@ -1511,7 +1526,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>194</v>
       </c>
@@ -1523,7 +1538,7 @@
       </c>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>194</v>
       </c>
@@ -1535,7 +1550,7 @@
       </c>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>194</v>
       </c>
@@ -2405,7 +2420,7 @@
       </c>
       <c r="D85" s="2"/>
     </row>
-    <row r="86" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>163</v>
       </c>
@@ -2415,9 +2430,11 @@
       <c r="C86" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D86" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>163</v>
       </c>
@@ -2427,9 +2444,11 @@
       <c r="C87" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D87" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>163</v>
       </c>
@@ -2439,9 +2458,11 @@
       <c r="C88" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D88" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>163</v>
       </c>
@@ -2451,9 +2472,11 @@
       <c r="C89" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D89" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>163</v>
       </c>
@@ -2463,9 +2486,11 @@
       <c r="C90" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D90" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>163</v>
       </c>
@@ -2475,9 +2500,11 @@
       <c r="C91" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D91" s="2" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>163</v>
       </c>
@@ -2487,7 +2514,9 @@
       <c r="C92" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="D92" s="2"/>
+      <c r="D92" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="93" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
@@ -3135,7 +3164,9 @@
       <c r="C146" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D146" s="2"/>
+      <c r="D146" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="147" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
@@ -3147,7 +3178,9 @@
       <c r="C147" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D147" s="2"/>
+      <c r="D147" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="148" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
@@ -3171,7 +3204,9 @@
       <c r="C149" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D149" s="2"/>
+      <c r="D149" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="150" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
@@ -3207,7 +3242,9 @@
       <c r="C152" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D152" s="2"/>
+      <c r="D152" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="153" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
@@ -3219,7 +3256,9 @@
       <c r="C153" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D153" s="2"/>
+      <c r="D153" s="2" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="154" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
@@ -3231,7 +3270,9 @@
       <c r="C154" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D154" s="2"/>
+      <c r="D154" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="155" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
@@ -3255,7 +3296,9 @@
       <c r="C156" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D156" s="2"/>
+      <c r="D156" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
@@ -3267,7 +3310,9 @@
       <c r="C157" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D157" s="2"/>
+      <c r="D157" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
@@ -3279,7 +3324,9 @@
       <c r="C158" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D158" s="2"/>
+      <c r="D158" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
@@ -3291,7 +3338,9 @@
       <c r="C159" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D159" s="2"/>
+      <c r="D159" s="2" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">

</xml_diff>

<commit_message>
Finished initial short params tests
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="617" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="275">
   <si>
     <t>Requirement</t>
   </si>
@@ -447,9 +447,6 @@
   </si>
   <si>
     <t>A GeogLinearUnitsGeoKey value of 32767 SHALL be a user-defined linear unit. If the value is 32767 (User-Defined) then the GeodeticCitationGeoKey and the GeogLinearUnitSizeGeoKey SHALL be populated</t>
-  </si>
-  <si>
-    <t>A ProjLinearUnitsGeoKey value of 32767 SHALL be a user-defined linear unit. If the value is 32767 (User-Defined) then the ProjectedCitationGeoKey and the ProjLinearUnitSizeGeoKey SHALL be populated.</t>
   </si>
   <si>
     <t>A VerticalUnitsGeoKey value of 32767 (user defined) SHALL not be used</t>
@@ -916,6 +913,9 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>A ProjLinearUnitsGeoKey value of 32767 SHALL be a user-defined linear unit. If the value is 32767 (User-Defined) then the ProjectedCitationGeoKey and the ProjLinearUnitSizeGeoKey SHALL be populated</t>
   </si>
 </sst>
 </file>
@@ -1013,7 +1013,7 @@
   <autoFilter ref="A1:D178">
     <filterColumn colId="0">
       <filters>
-        <filter val="requirements_class_ProjMethodGeoKey"/>
+        <filter val="requirements_class_VerticalDatumGeoKey"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1296,8 +1296,8 @@
   <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E133" sqref="E133:F133"/>
+      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E183" sqref="E183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1310,7 +1310,7 @@
   <sheetData>
     <row r="1" spans="1:4" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1384,181 +1384,181 @@
     </row>
     <row r="7" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B8" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>184</v>
-      </c>
       <c r="D8" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>180</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>181</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="C13" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>202</v>
       </c>
       <c r="D13" s="2"/>
     </row>
     <row r="14" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>192</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>193</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="C16" s="3" t="s">
         <v>189</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>190</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>198</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>199</v>
       </c>
       <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -1633,7 +1633,7 @@
         <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1647,7 +1647,7 @@
         <v>102</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1661,7 +1661,7 @@
         <v>102</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1675,7 +1675,7 @@
         <v>102</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -1689,7 +1689,7 @@
         <v>102</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1703,7 +1703,7 @@
         <v>99</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1717,105 +1717,105 @@
         <v>99</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B35" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>158</v>
-      </c>
       <c r="D35" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B38" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="C38" s="3" t="s">
         <v>154</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>155</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1897,7 +1897,7 @@
         <v>13</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1911,7 +1911,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1925,7 +1925,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1939,7 +1939,7 @@
         <v>13</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1953,7 +1953,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1967,7 +1967,7 @@
         <v>13</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -2005,7 +2005,7 @@
         <v>16</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2019,7 +2019,7 @@
         <v>16</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2033,7 +2033,7 @@
         <v>16</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2047,7 +2047,7 @@
         <v>16</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2061,7 +2061,7 @@
         <v>16</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2075,7 +2075,7 @@
         <v>16</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2113,7 +2113,7 @@
         <v>65</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2127,7 +2127,7 @@
         <v>65</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2141,7 +2141,7 @@
         <v>65</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2155,7 +2155,7 @@
         <v>65</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2169,7 +2169,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2183,7 +2183,7 @@
         <v>65</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2197,7 +2197,7 @@
         <v>63</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2211,7 +2211,7 @@
         <v>63</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2225,7 +2225,7 @@
         <v>6</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2233,13 +2233,13 @@
         <v>60</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2253,7 +2253,7 @@
         <v>57</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2267,7 +2267,7 @@
         <v>57</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2281,7 +2281,7 @@
         <v>55</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2295,7 +2295,7 @@
         <v>55</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
@@ -2303,13 +2303,13 @@
         <v>53</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2422,303 +2422,303 @@
     </row>
     <row r="86" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B87" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B88" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B89" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="C89" s="3" t="s">
         <v>167</v>
       </c>
-      <c r="C89" s="3" t="s">
-        <v>168</v>
-      </c>
       <c r="D89" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B91" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="B91" s="3" t="s">
+      <c r="C91" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="C91" s="3" t="s">
-        <v>165</v>
-      </c>
       <c r="D91" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B93" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="C93" s="3" t="s">
         <v>177</v>
-      </c>
-      <c r="C93" s="3" t="s">
-        <v>178</v>
       </c>
       <c r="D93" s="2"/>
     </row>
     <row r="94" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="B94" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B94" s="3" t="s">
+      <c r="C94" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="C94" s="3" t="s">
-        <v>175</v>
       </c>
       <c r="D94" s="2"/>
     </row>
     <row r="95" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D95" s="2"/>
     </row>
     <row r="96" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>243</v>
-      </c>
-      <c r="C96" s="3" t="s">
-        <v>244</v>
       </c>
       <c r="D96" s="2"/>
     </row>
     <row r="97" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D97" s="2"/>
     </row>
     <row r="98" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D98" s="2"/>
     </row>
     <row r="99" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D99" s="2"/>
     </row>
     <row r="100" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D100" s="2"/>
     </row>
     <row r="101" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D101" s="2"/>
     </row>
     <row r="102" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D102" s="2"/>
     </row>
     <row r="103" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D103" s="2"/>
     </row>
     <row r="104" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>232</v>
-      </c>
-      <c r="C104" s="3" t="s">
-        <v>233</v>
       </c>
       <c r="D104" s="2"/>
     </row>
     <row r="105" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D105" s="2"/>
     </row>
     <row r="106" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D106" s="2"/>
     </row>
     <row r="107" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="C107" s="3" t="s">
-        <v>250</v>
       </c>
       <c r="D107" s="2"/>
     </row>
     <row r="108" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>246</v>
-      </c>
-      <c r="C108" s="3" t="s">
-        <v>247</v>
       </c>
       <c r="D108" s="2"/>
     </row>
     <row r="109" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D109" s="2"/>
     </row>
@@ -2733,7 +2733,7 @@
         <v>92</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2747,7 +2747,7 @@
         <v>92</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2761,7 +2761,7 @@
         <v>92</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2775,7 +2775,7 @@
         <v>92</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2789,7 +2789,7 @@
         <v>92</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2803,7 +2803,7 @@
         <v>89</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2817,306 +2817,306 @@
         <v>89</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B117" s="3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C117" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B118" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C118" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B119" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="C119" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="C119" s="3" t="s">
-        <v>218</v>
-      </c>
       <c r="D119" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B120" s="3" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="B121" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B121" s="3" t="s">
+      <c r="C121" s="3" t="s">
         <v>214</v>
       </c>
-      <c r="C121" s="3" t="s">
-        <v>215</v>
-      </c>
       <c r="D121" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="123" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>261</v>
-      </c>
-      <c r="C123" s="3" t="s">
-        <v>262</v>
       </c>
       <c r="D123" s="2"/>
     </row>
     <row r="124" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D124" s="2"/>
     </row>
     <row r="125" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D125" s="2"/>
     </row>
     <row r="126" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D126" s="2"/>
     </row>
     <row r="127" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="B127" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="C127" s="3" t="s">
         <v>252</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>253</v>
       </c>
       <c r="D127" s="2"/>
     </row>
     <row r="128" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D128" s="2"/>
     </row>
     <row r="129" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B129" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>255</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>256</v>
       </c>
       <c r="D129" s="2"/>
     </row>
     <row r="130" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D130" s="2"/>
     </row>
-    <row r="131" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B131" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D131" s="2" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A132" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="133" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B133" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D133" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="134" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B135" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="B131" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A132" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B132" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="133" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A133" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B133" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="C133" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D133" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="134" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A134" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B134" s="3" t="s">
-        <v>230</v>
-      </c>
-      <c r="C134" s="3" t="s">
-        <v>227</v>
-      </c>
-      <c r="D134" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="135" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A135" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B135" s="3" t="s">
+      <c r="C135" s="3" t="s">
         <v>223</v>
       </c>
-      <c r="C135" s="3" t="s">
+      <c r="D135" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="136" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="B136" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="D135" s="2" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A136" s="3" t="s">
-        <v>222</v>
-      </c>
-      <c r="B136" s="3" t="s">
-        <v>225</v>
-      </c>
       <c r="C136" s="3" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D137" s="2"/>
     </row>
     <row r="138" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D138" s="2"/>
     </row>
     <row r="139" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>264</v>
-      </c>
-      <c r="C139" s="3" t="s">
-        <v>265</v>
       </c>
       <c r="D139" s="2"/>
     </row>
@@ -3203,7 +3203,7 @@
         <v>128</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3217,7 +3217,7 @@
         <v>128</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3231,7 +3231,7 @@
         <v>128</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3245,7 +3245,7 @@
         <v>128</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3258,7 +3258,9 @@
       <c r="C150" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D150" s="2"/>
+      <c r="D150" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="151" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
@@ -3270,7 +3272,9 @@
       <c r="C151" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="D151" s="2"/>
+      <c r="D151" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="152" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
@@ -3283,7 +3287,7 @@
         <v>135</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3297,7 +3301,7 @@
         <v>135</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3305,13 +3309,13 @@
         <v>126</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>140</v>
+        <v>274</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3319,12 +3323,14 @@
         <v>126</v>
       </c>
       <c r="B155" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C155" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="D155" s="2"/>
+      <c r="D155" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="156" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
@@ -3337,7 +3343,7 @@
         <v>135</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3351,7 +3357,7 @@
         <v>135</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3359,13 +3365,13 @@
         <v>126</v>
       </c>
       <c r="B158" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C158" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3379,164 +3385,176 @@
         <v>135</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="B160" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="B160" s="3" t="s">
+      <c r="C160" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="C160" s="3" t="s">
-        <v>145</v>
       </c>
       <c r="D160" s="2"/>
     </row>
     <row r="161" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B161" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C161" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D161" s="2"/>
     </row>
     <row r="162" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B162" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C162" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D162" s="2"/>
     </row>
     <row r="163" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B163" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D163" s="2"/>
     </row>
     <row r="164" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B164" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C164" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="C164" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="D164" s="2"/>
     </row>
     <row r="165" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B165" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D165" s="2"/>
     </row>
     <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D166" s="2"/>
     </row>
-    <row r="167" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B167" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="B167" s="3" t="s">
+      <c r="C167" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="C167" s="3" t="s">
+      <c r="D167" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A168" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B168" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="D167" s="2"/>
-    </row>
-    <row r="168" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B168" s="3" t="s">
+      <c r="C168" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="D168" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A169" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D169" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A170" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D170" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A171" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B171" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="C168" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="D168" s="2"/>
-    </row>
-    <row r="169" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B169" s="3" t="s">
+      <c r="C171" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="D171" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A172" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="B172" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="C169" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D169" s="2"/>
-    </row>
-    <row r="170" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B170" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="C170" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D170" s="2"/>
-    </row>
-    <row r="171" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B171" s="3" t="s">
+      <c r="C172" s="3" t="s">
         <v>208</v>
       </c>
-      <c r="C171" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D171" s="2"/>
-    </row>
-    <row r="172" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="B172" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="C172" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="D172" s="2"/>
+      <c r="D172" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="173" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
@@ -3548,7 +3566,9 @@
       <c r="C173" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D173" s="2"/>
+      <c r="D173" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="174" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
@@ -3560,7 +3580,9 @@
       <c r="C174" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="D174" s="2"/>
+      <c r="D174" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="175" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
@@ -3572,19 +3594,23 @@
       <c r="C175" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D175" s="2"/>
+      <c r="D175" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="176" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D176" s="2"/>
+      <c r="D176" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="177" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
@@ -3596,7 +3622,9 @@
       <c r="C177" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D177" s="2"/>
+      <c r="D177" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="178" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
@@ -3608,7 +3636,9 @@
       <c r="C178" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="D178" s="2"/>
+      <c r="D178" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Restructure params. Might have to begin implementing ListGeo
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="275">
   <si>
     <t>Requirement</t>
   </si>
@@ -1011,9 +1011,20 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D178">
-    <filterColumn colId="0">
+    <filterColumn colId="1">
       <filters>
-        <filter val="requirements_class_VerticalDatumGeoKey"/>
+        <filter val="A GeogLinearUnitsGeoKey value of 32767 SHALL be a user-defined linear unit. If the value is 32767 (User-Defined) then the GeodeticCitationGeoKey and the GeogLinearUnitSizeGeoKey SHALL be populated"/>
+        <filter val="GeogAngularUnitsGeoKey, GeogAzimuthUnitsGeoKey, GeogLinearUnitsGeoKey, ProjLinearUnitsGeoKey and VerticalUnitsGeoKey values in the range 1-1023 SHALL be reserved."/>
+        <filter val="GeogAngularUnitsGeoKey, GeogAzimuthUnitsGeoKey, GeogLinearUnitsGeoKey, ProjLinearUnitsGeoKey and VerticalUnitsGeoKey values in the range 32768-65535 SHALL be private."/>
+        <filter val="GeogLinearUnitsGeoKey, ProjLinearUnitsGeoKey and VerticalUnitsGeoKey values in the range 1024-32766 SHALL be EPSG Unit Of Measure (UOM) codes with type = length."/>
+        <filter val="If the GeodeticCRSGeoKey value is 32767 (User-Defined) then the GeodeticCitationGeoKey, GeodeticDatumGeoKey and at least one of GeogAngularUnitsGeoKey or GeogLinearUnitsGeoKey SHALL be populated."/>
+        <filter val="The GeogAngularUnitsGeoKey, the GeogAzimuthUnitsGeoKey, the GeogLinearUnitsGeoKey, the ProjLinearUnitsGeoKey and the VerticalUnitsGeoKey SHALL each have type = SHORT"/>
+        <filter val="The GeogAngularUnitSizeGeoKey, GeogLinearUnitSizeGeoKey and ProjLinearUnitSizeGeoKey SHALL each have type = DOUBLE"/>
+        <filter val="The GeogLinearUnitsGeoKey SHALL have ID = 2052"/>
+        <filter val="The GeogLinearUnitSizeGeoKey SHALL have ID = 2053"/>
+        <filter val="The units of the EllipsoidSemiMajorAxisGeoKey SHALL be defined by the value of GeogLinearUnitsGeoKey"/>
+        <filter val="The units of the EllipsoidSemiMinorAxisGeoKey SHALL be defined by the value of GeogLinearUnitsGeoKey"/>
+        <filter val="The units of the GeogLinearUnitSizeGeoKey value SHALL be meters."/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1296,8 +1307,8 @@
   <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E183" sqref="E183"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C181" sqref="C181"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1490,7 +1501,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>187</v>
       </c>
@@ -1526,7 +1537,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>193</v>
       </c>
@@ -1678,7 +1689,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>97</v>
       </c>
@@ -3206,7 +3217,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>126</v>
       </c>
@@ -3234,7 +3245,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>126</v>
       </c>
@@ -3290,7 +3301,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
         <v>126</v>
       </c>
@@ -3346,7 +3357,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>126</v>
       </c>
@@ -3360,7 +3371,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>126</v>
       </c>
@@ -3374,7 +3385,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>126</v>
       </c>
@@ -3400,7 +3411,7 @@
       </c>
       <c r="D160" s="2"/>
     </row>
-    <row r="161" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
         <v>142</v>
       </c>
@@ -3412,7 +3423,7 @@
       </c>
       <c r="D161" s="2"/>
     </row>
-    <row r="162" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
         <v>142</v>
       </c>
@@ -3422,7 +3433,9 @@
       <c r="C162" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D162" s="2"/>
+      <c r="D162" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="163" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
@@ -3448,7 +3461,7 @@
       </c>
       <c r="D164" s="2"/>
     </row>
-    <row r="165" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
         <v>142</v>
       </c>
@@ -3472,7 +3485,7 @@
       </c>
       <c r="D166" s="2"/>
     </row>
-    <row r="167" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>203</v>
       </c>
@@ -3486,7 +3499,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>203</v>
       </c>
@@ -3500,7 +3513,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
         <v>203</v>
       </c>
@@ -3514,7 +3527,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
         <v>203</v>
       </c>
@@ -3528,7 +3541,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
         <v>203</v>
       </c>
@@ -3542,7 +3555,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
         <v>203</v>
       </c>

</xml_diff>

<commit_message>
Intgration of EPSG code testing into Double, Short params
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="275">
   <si>
     <t>Requirement</t>
   </si>
@@ -1013,18 +1013,10 @@
   <autoFilter ref="A1:D178">
     <filterColumn colId="1">
       <filters>
-        <filter val="A GeogLinearUnitsGeoKey value of 32767 SHALL be a user-defined linear unit. If the value is 32767 (User-Defined) then the GeodeticCitationGeoKey and the GeogLinearUnitSizeGeoKey SHALL be populated"/>
-        <filter val="GeogAngularUnitsGeoKey, GeogAzimuthUnitsGeoKey, GeogLinearUnitsGeoKey, ProjLinearUnitsGeoKey and VerticalUnitsGeoKey values in the range 1-1023 SHALL be reserved."/>
-        <filter val="GeogAngularUnitsGeoKey, GeogAzimuthUnitsGeoKey, GeogLinearUnitsGeoKey, ProjLinearUnitsGeoKey and VerticalUnitsGeoKey values in the range 32768-65535 SHALL be private."/>
-        <filter val="GeogLinearUnitsGeoKey, ProjLinearUnitsGeoKey and VerticalUnitsGeoKey values in the range 1024-32766 SHALL be EPSG Unit Of Measure (UOM) codes with type = length."/>
-        <filter val="If the GeodeticCRSGeoKey value is 32767 (User-Defined) then the GeodeticCitationGeoKey, GeodeticDatumGeoKey and at least one of GeogAngularUnitsGeoKey or GeogLinearUnitsGeoKey SHALL be populated."/>
-        <filter val="The GeogAngularUnitsGeoKey, the GeogAzimuthUnitsGeoKey, the GeogLinearUnitsGeoKey, the ProjLinearUnitsGeoKey and the VerticalUnitsGeoKey SHALL each have type = SHORT"/>
+        <filter val="A GeogAngularUnitsGeoKey or a GeogAzimuthUnitsGeoKey value of 32767 SHALL be a user-defined angular unit. If the value is 32767 (User-Defined) then the GeodeticCitationGeoKey and the GeogAngularUnitSizeGeoKey SHALL be populated"/>
+        <filter val="The GeogAngularUnitSizeGeoKey SHALL have ID = 2055"/>
         <filter val="The GeogAngularUnitSizeGeoKey, GeogLinearUnitSizeGeoKey and ProjLinearUnitSizeGeoKey SHALL each have type = DOUBLE"/>
-        <filter val="The GeogLinearUnitsGeoKey SHALL have ID = 2052"/>
-        <filter val="The GeogLinearUnitSizeGeoKey SHALL have ID = 2053"/>
-        <filter val="The units of the EllipsoidSemiMajorAxisGeoKey SHALL be defined by the value of GeogLinearUnitsGeoKey"/>
-        <filter val="The units of the EllipsoidSemiMinorAxisGeoKey SHALL be defined by the value of GeogLinearUnitsGeoKey"/>
-        <filter val="The units of the GeogLinearUnitSizeGeoKey value SHALL be meters."/>
+        <filter val="The units of the GeogAngularUnitSizeGeoKey value SHALL be radians."/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1307,8 +1299,8 @@
   <dimension ref="A1:D178"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A153" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B165" sqref="B165"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G164" sqref="G164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1501,7 +1493,7 @@
       </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>187</v>
       </c>
@@ -1537,7 +1529,7 @@
       </c>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>193</v>
       </c>
@@ -1689,7 +1681,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>97</v>
       </c>
@@ -3217,7 +3209,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>126</v>
       </c>
@@ -3245,7 +3237,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>126</v>
       </c>
@@ -3287,7 +3279,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
         <v>126</v>
       </c>
@@ -3301,7 +3293,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
         <v>126</v>
       </c>
@@ -3357,7 +3349,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>126</v>
       </c>
@@ -3371,7 +3363,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>126</v>
       </c>
@@ -3385,7 +3377,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>126</v>
       </c>
@@ -3399,7 +3391,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
         <v>142</v>
       </c>
@@ -3409,7 +3401,9 @@
       <c r="C160" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D160" s="2"/>
+      <c r="D160" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="161" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
@@ -3421,9 +3415,11 @@
       <c r="C161" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="D161" s="2"/>
-    </row>
-    <row r="162" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D161" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
         <v>142</v>
       </c>
@@ -3449,7 +3445,7 @@
       </c>
       <c r="D163" s="2"/>
     </row>
-    <row r="164" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
         <v>142</v>
       </c>
@@ -3459,9 +3455,11 @@
       <c r="C164" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D164" s="2"/>
-    </row>
-    <row r="165" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D164" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
         <v>142</v>
       </c>
@@ -3471,7 +3469,9 @@
       <c r="C165" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="D165" s="2"/>
+      <c r="D165" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">

</xml_diff>

<commit_message>
Implemented EPSG tables for shortparams
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14388"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="4872"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Trace Matrix" sheetId="1" r:id="rId1"/>
@@ -1011,12 +1011,23 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D178">
-    <filterColumn colId="1">
+    <filterColumn colId="2">
       <filters>
-        <filter val="A GeogAngularUnitsGeoKey or a GeogAzimuthUnitsGeoKey value of 32767 SHALL be a user-defined angular unit. If the value is 32767 (User-Defined) then the GeodeticCitationGeoKey and the GeogAngularUnitSizeGeoKey SHALL be populated"/>
-        <filter val="The GeogAngularUnitSizeGeoKey SHALL have ID = 2055"/>
-        <filter val="The GeogAngularUnitSizeGeoKey, GeogLinearUnitSizeGeoKey and ProjLinearUnitSizeGeoKey SHALL each have type = DOUBLE"/>
-        <filter val="The units of the GeogAngularUnitSizeGeoKey value SHALL be radians."/>
+        <filter val="TIFF_Test/DoubleParameters, TIFF_Test/AsciiParameters, TIFF_Test/ShortParameters"/>
+        <filter val="TIFF_Test/GeoKeyDirectory, TIFF_Test/DoubleParameters, TIFF_Test/AsciiParameters, TIFF_Test/ShortParameters"/>
+        <filter val="TIFF_Test/ShortParameters"/>
+        <filter val="TIFF_Test/ShortParameters, Configuration_GeoKey/GTModelTypeGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Configuration_GeoKey/GTRasterTypeGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Geodetic_CRS_GeoKey/EllipsoidGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Geodetic_CRS_GeoKey/GeodeticCRSGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Geodetic_CRS_GeoKey/GeodeticDatumGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Geodetic_CRS_GeoKey/PrimeMeridianGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Projection_CRS_GeoKey/ProjectedCRSGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Projection_Definition_GeoKey/ProjectionGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Projection_Definition_GeoKey/ProjMethodGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Units_GeoKeys/UnitsGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Vertical_GeoKeys/VerticalDatumGeoKey"/>
+        <filter val="TIFF_Test/ShortParameters, Vertical_GeoKeys/VerticalGeoKey"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1298,9 +1309,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G164" sqref="G164"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1441,7 +1452,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>178</v>
       </c>
@@ -1455,7 +1466,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>178</v>
       </c>
@@ -1695,7 +1706,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>97</v>
       </c>
@@ -1709,7 +1720,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>97</v>
       </c>
@@ -1793,7 +1804,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>152</v>
       </c>
@@ -1807,7 +1818,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>152</v>
       </c>
@@ -1865,7 +1876,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -1877,7 +1888,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -1973,7 +1984,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>14</v>
       </c>
@@ -1985,7 +1996,7 @@
       </c>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
@@ -2081,7 +2092,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -2093,7 +2104,7 @@
       </c>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -2189,7 +2200,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>60</v>
       </c>
@@ -2203,7 +2214,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>60</v>
       </c>
@@ -2273,7 +2284,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>53</v>
       </c>
@@ -2287,7 +2298,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>53</v>
       </c>
@@ -2493,7 +2504,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>162</v>
       </c>
@@ -2507,7 +2518,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="92" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>162</v>
       </c>
@@ -2795,7 +2806,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>87</v>
       </c>
@@ -2809,7 +2820,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="116" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>87</v>
       </c>
@@ -2879,7 +2890,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>212</v>
       </c>
@@ -2893,7 +2904,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>212</v>
       </c>
@@ -3059,7 +3070,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>221</v>
       </c>
@@ -3073,7 +3084,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>221</v>
       </c>
@@ -3195,7 +3206,7 @@
       </c>
       <c r="D145" s="2"/>
     </row>
-    <row r="146" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>126</v>
       </c>
@@ -3209,7 +3220,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="147" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>126</v>
       </c>
@@ -3220,10 +3231,10 @@
         <v>128</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="148" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="148" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>126</v>
       </c>
@@ -3237,7 +3248,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="149" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>126</v>
       </c>
@@ -3251,7 +3262,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="150" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>126</v>
       </c>
@@ -3265,7 +3276,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="151" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
         <v>126</v>
       </c>
@@ -3279,7 +3290,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="152" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
         <v>126</v>
       </c>
@@ -3391,7 +3402,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="160" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
         <v>142</v>
       </c>
@@ -3405,7 +3416,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
         <v>142</v>
       </c>
@@ -3445,7 +3456,7 @@
       </c>
       <c r="D163" s="2"/>
     </row>
-    <row r="164" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
         <v>142</v>
       </c>
@@ -3485,7 +3496,7 @@
       </c>
       <c r="D166" s="2"/>
     </row>
-    <row r="167" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>203</v>
       </c>
@@ -3499,7 +3510,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>203</v>
       </c>
@@ -3569,7 +3580,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
         <v>107</v>
       </c>
@@ -3583,7 +3594,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
         <v>107</v>
       </c>

</xml_diff>

<commit_message>
DoubleParams fix, initial AsciiParams
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="277">
   <si>
     <t>Requirement</t>
   </si>
@@ -1019,10 +1019,7 @@
   <autoFilter ref="A1:D178">
     <filterColumn colId="0">
       <filters>
-        <filter val="requirements_class_EllipsoidGeoKey"/>
-        <filter val="requirements_class_EllipsoidInvFlatteningGeoKey"/>
-        <filter val="requirements_class_EllipsoidSemiMajorAxisGeoKey"/>
-        <filter val="requirements_class_EllipsoidSemiMinorAxisGeoKey"/>
+        <filter val="requirements_class_CitationGeoKeys"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1305,8 +1302,8 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1331,7 +1328,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1343,7 +1340,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>115</v>
       </c>
@@ -1353,9 +1350,11 @@
       <c r="C3" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="4" spans="1:4" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D3" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>115</v>
       </c>
@@ -1365,9 +1364,11 @@
       <c r="C4" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D4" s="2"/>
-    </row>
-    <row r="5" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D4" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>115</v>
       </c>
@@ -1379,7 +1380,7 @@
       </c>
       <c r="D5" s="2"/>
     </row>
-    <row r="6" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>115</v>
       </c>
@@ -1391,7 +1392,7 @@
       </c>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>178</v>
       </c>
@@ -1405,7 +1406,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>178</v>
       </c>
@@ -1419,7 +1420,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>178</v>
       </c>
@@ -1433,7 +1434,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>178</v>
       </c>
@@ -1447,7 +1448,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>178</v>
       </c>
@@ -1461,7 +1462,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>178</v>
       </c>
@@ -1475,7 +1476,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>199</v>
       </c>
@@ -1489,7 +1490,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>199</v>
       </c>
@@ -1503,7 +1504,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>187</v>
       </c>
@@ -1517,7 +1518,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>187</v>
       </c>
@@ -1531,7 +1532,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>187</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>193</v>
       </c>
@@ -1559,7 +1560,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>193</v>
       </c>
@@ -1573,7 +1574,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>193</v>
       </c>
@@ -3735,7 +3736,7 @@
       </c>
       <c r="G180">
         <f>COUNTIF(D:D, "D")</f>
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -3744,7 +3745,7 @@
       </c>
       <c r="G181">
         <f xml:space="preserve"> 178 - G180</f>
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
GeoAsciiParamsTag tests added. Fixed escape char issue.
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="277">
   <si>
     <t>Requirement</t>
   </si>
@@ -1017,10 +1017,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D178">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="The GeodeticCitationGeoKey SHALL have ID = 2049"/>
-      </filters>
+    <filterColumn colId="3">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:D187">
@@ -1302,8 +1300,8 @@
   <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D187" sqref="D187"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1328,7 +1326,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1594,7 +1592,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1604,9 +1602,11 @@
       <c r="C21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D21" s="2"/>
-    </row>
-    <row r="22" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D21" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1616,9 +1616,11 @@
       <c r="C22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D22" s="2"/>
-    </row>
-    <row r="23" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D22" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1628,9 +1630,11 @@
       <c r="C23" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="2"/>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D23" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1642,7 +1646,7 @@
       </c>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -1652,7 +1656,9 @@
       <c r="C25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="2"/>
+      <c r="D25" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
@@ -1850,7 +1856,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1862,7 +1868,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -1874,7 +1880,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
@@ -1884,7 +1890,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" ht="15.6" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
@@ -1894,7 +1900,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -1906,7 +1912,7 @@
       </c>
       <c r="D44" s="2"/>
     </row>
-    <row r="45" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>14</v>
       </c>
@@ -2014,7 +2020,7 @@
       </c>
       <c r="D52" s="2"/>
     </row>
-    <row r="53" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
@@ -2110,7 +2116,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -2122,7 +2128,7 @@
       </c>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -2344,7 +2350,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
@@ -2356,7 +2362,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>77</v>
       </c>
@@ -2368,7 +2374,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>77</v>
       </c>
@@ -2380,7 +2386,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -2392,7 +2398,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>72</v>
       </c>
@@ -2404,7 +2410,7 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>72</v>
       </c>
@@ -2416,7 +2422,7 @@
       </c>
       <c r="D82" s="2"/>
     </row>
-    <row r="83" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
@@ -2428,7 +2434,7 @@
       </c>
       <c r="D83" s="2"/>
     </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>82</v>
       </c>
@@ -2440,7 +2446,7 @@
       </c>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>82</v>
       </c>
@@ -2746,7 +2752,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>244</v>
       </c>
@@ -2758,7 +2764,7 @@
       </c>
       <c r="D107" s="2"/>
     </row>
-    <row r="108" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>244</v>
       </c>
@@ -2770,7 +2776,7 @@
       </c>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>244</v>
       </c>
@@ -3202,7 +3208,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>2</v>
       </c>
@@ -3214,7 +3220,7 @@
       </c>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>2</v>
       </c>
@@ -3226,7 +3232,7 @@
       </c>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>2</v>
       </c>
@@ -3238,7 +3244,7 @@
       </c>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>2</v>
       </c>
@@ -3250,7 +3256,7 @@
       </c>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>2</v>
       </c>
@@ -3262,7 +3268,7 @@
       </c>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>2</v>
       </c>
@@ -3742,7 +3748,7 @@
       </c>
       <c r="G180">
         <f>COUNTIF(D:D, "D")</f>
-        <v>130</v>
+        <v>134</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -3751,7 +3757,7 @@
       </c>
       <c r="G181">
         <f xml:space="preserve"> 178 - G180</f>
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Various fixes, comments, and refactoring
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="278">
   <si>
     <t>Requirement</t>
   </si>
@@ -922,6 +922,9 @@
   </si>
   <si>
     <t>Left:</t>
+  </si>
+  <si>
+    <t>Partial:</t>
   </si>
 </sst>
 </file>
@@ -1017,8 +1020,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D178">
-    <filterColumn colId="3">
-      <filters blank="1"/>
+    <filterColumn colId="0">
+      <filters>
+        <filter val="requirements_class_ModelTransformationTag"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:D187">
@@ -1297,11 +1302,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G181"/>
+  <dimension ref="A1:G182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F185" sqref="F185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1592,7 +1597,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1606,7 +1611,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1620,7 +1625,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1634,7 +1639,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1644,9 +1649,11 @@
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="2"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D24" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -1856,7 +1863,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1868,7 +1875,7 @@
       </c>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -1880,7 +1887,7 @@
       </c>
       <c r="D41" s="2"/>
     </row>
-    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
@@ -1890,7 +1897,7 @@
       <c r="C42" s="3"/>
       <c r="D42" s="2"/>
     </row>
-    <row r="43" spans="1:4" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
@@ -1900,7 +1907,7 @@
       <c r="C43" s="3"/>
       <c r="D43" s="2"/>
     </row>
-    <row r="44" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -1910,9 +1917,11 @@
       <c r="C44" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D44" s="2"/>
-    </row>
-    <row r="45" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D44" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -1922,7 +1931,9 @@
       <c r="C45" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D45" s="2"/>
+      <c r="D45" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="46" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
@@ -2008,7 +2019,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>14</v>
       </c>
@@ -2018,9 +2029,11 @@
       <c r="C52" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D52" s="2"/>
-    </row>
-    <row r="53" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="D52" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
@@ -2030,7 +2043,9 @@
       <c r="C53" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D53" s="2"/>
+      <c r="D53" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="54" spans="1:4" ht="32.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
@@ -2116,7 +2131,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -2128,7 +2143,7 @@
       </c>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -2350,7 +2365,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
@@ -2362,7 +2377,7 @@
       </c>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>77</v>
       </c>
@@ -2374,7 +2389,7 @@
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>77</v>
       </c>
@@ -2384,9 +2399,11 @@
       <c r="C79" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D79" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -2398,7 +2415,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>72</v>
       </c>
@@ -2410,7 +2427,7 @@
       </c>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>72</v>
       </c>
@@ -2420,7 +2437,9 @@
       <c r="C82" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D82" s="2"/>
+      <c r="D82" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
@@ -2432,7 +2451,9 @@
       <c r="C83" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D83" s="2"/>
+      <c r="D83" s="2" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
@@ -2456,7 +2477,9 @@
       <c r="C85" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D85" s="2"/>
+      <c r="D85" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="86" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
@@ -2752,7 +2775,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>244</v>
       </c>
@@ -2762,9 +2785,11 @@
       <c r="C107" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D107" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>244</v>
       </c>
@@ -2774,9 +2799,11 @@
       <c r="C108" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D108" s="2"/>
-    </row>
-    <row r="109" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="D108" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>244</v>
       </c>
@@ -2786,7 +2813,9 @@
       <c r="C109" s="3" t="s">
         <v>246</v>
       </c>
-      <c r="D109" s="2"/>
+      <c r="D109" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="110" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
@@ -3208,7 +3237,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>2</v>
       </c>
@@ -3220,7 +3249,7 @@
       </c>
       <c r="D140" s="2"/>
     </row>
-    <row r="141" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>2</v>
       </c>
@@ -3232,7 +3261,7 @@
       </c>
       <c r="D141" s="2"/>
     </row>
-    <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>2</v>
       </c>
@@ -3244,7 +3273,7 @@
       </c>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>2</v>
       </c>
@@ -3256,7 +3285,7 @@
       </c>
       <c r="D143" s="2"/>
     </row>
-    <row r="144" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>2</v>
       </c>
@@ -3268,7 +3297,7 @@
       </c>
       <c r="D144" s="2"/>
     </row>
-    <row r="145" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>2</v>
       </c>
@@ -3278,7 +3307,9 @@
       <c r="C145" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D145" s="2"/>
+      <c r="D145" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="146" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
@@ -3748,16 +3779,25 @@
       </c>
       <c r="G180">
         <f>COUNTIF(D:D, "D")</f>
-        <v>134</v>
+        <v>145</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F181" t="s">
+        <v>277</v>
+      </c>
+      <c r="G181">
+        <f>COUNTIF(D:D, "P")</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F182" t="s">
         <v>276</v>
       </c>
-      <c r="G181">
-        <f xml:space="preserve"> 178 - G180</f>
-        <v>44</v>
+      <c r="G182">
+        <f xml:space="preserve"> 178 - G180 -G181</f>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completing various geokey requirements
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="279">
   <si>
     <t>Requirement</t>
   </si>
@@ -878,6 +878,39 @@
     </r>
   </si>
   <si>
+    <t>The GTRasterTypeGeoKey value SHALL be
+- 0 to indicate that the Raster type is undefined or unknown; or
+- 1 to indidate that the Raster type is PixelIsArea; or
+- 2 to indicate that the Raster type is PixelIsPoint; or
+- 32767 to indicate that the Raster type is user-defined</t>
+  </si>
+  <si>
+    <t>The GTModelTypeGeoKey value SHALL be:
+- 0 to indicate that the Model CRS is undefined or unknown
+- 1 to indicate that the Model CRS is a 2D projected Coordinate Reference System, indicated by the value of the ProjectedCRSGeoKey; or
+- 2 to indicate that the Model CRS is a 2DD geographic coordinate reference system, indicated by the value of the GeodeticCRSGeoKey; or
+- 3 to indicate that the Model CRS is a geocentric Cartesian 3D coordinate reference system, indicated by the value of the GeodeticCRSGeoKey; or
+- 32767 to indicate that the Model CRS type is user-defined.</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>A ProjLinearUnitsGeoKey value of 32767 SHALL be a user-defined linear unit. If the value is 32767 (User-Defined) then the ProjectedCitationGeoKey and the ProjLinearUnitSizeGeoKey SHALL be populated</t>
+  </si>
+  <si>
+    <t>Done:</t>
+  </si>
+  <si>
+    <t>Left:</t>
+  </si>
+  <si>
+    <t>Partial:</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Status
 </t>
@@ -890,41 +923,11 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>(D)one, (P)artial, Need (H)elp</t>
+      <t>(D)one, (P)artial, Need (H)elp, (N)ot Required</t>
     </r>
   </si>
   <si>
-    <t>The GTRasterTypeGeoKey value SHALL be
-- 0 to indicate that the Raster type is undefined or unknown; or
-- 1 to indidate that the Raster type is PixelIsArea; or
-- 2 to indicate that the Raster type is PixelIsPoint; or
-- 32767 to indicate that the Raster type is user-defined</t>
-  </si>
-  <si>
-    <t>The GTModelTypeGeoKey value SHALL be:
-- 0 to indicate that the Model CRS is undefined or unknown
-- 1 to indicate that the Model CRS is a 2D projected Coordinate Reference System, indicated by the value of the ProjectedCRSGeoKey; or
-- 2 to indicate that the Model CRS is a 2DD geographic coordinate reference system, indicated by the value of the GeodeticCRSGeoKey; or
-- 3 to indicate that the Model CRS is a geocentric Cartesian 3D coordinate reference system, indicated by the value of the GeodeticCRSGeoKey; or
-- 32767 to indicate that the Model CRS type is user-defined.</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>A ProjLinearUnitsGeoKey value of 32767 SHALL be a user-defined linear unit. If the value is 32767 (User-Defined) then the ProjectedCitationGeoKey and the ProjLinearUnitSizeGeoKey SHALL be populated</t>
-  </si>
-  <si>
-    <t>Done:</t>
-  </si>
-  <si>
-    <t>Left:</t>
-  </si>
-  <si>
-    <t>Partial:</t>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -1020,10 +1023,8 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D178">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="Requirements_class_GTModelTypeGeoKey"/>
-      </filters>
+    <filterColumn colId="3">
+      <filters blank="1"/>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:D187">
@@ -1033,7 +1034,7 @@
     <tableColumn id="1" name="Class" dataDxfId="3"/>
     <tableColumn id="2" name="Requirement" dataDxfId="2"/>
     <tableColumn id="3" name="Test" dataDxfId="1"/>
-    <tableColumn id="4" name="Status_x000a_(D)one, (P)artial, Need (H)elp" dataDxfId="0"/>
+    <tableColumn id="4" name="Status_x000a_(D)one, (P)artial, Need (H)elp, (N)ot Required" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1306,7 +1307,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F71" sqref="F71"/>
+      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1314,7 +1315,7 @@
     <col min="1" max="1" width="55.88671875" customWidth="1"/>
     <col min="2" max="2" width="56.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.6" x14ac:dyDescent="0.3">
@@ -1328,7 +1329,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>269</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1650,7 +1651,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1873,7 +1874,9 @@
       <c r="C40" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D40" s="2"/>
+      <c r="D40" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="41" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
@@ -1885,9 +1888,11 @@
       <c r="C41" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D41" s="2"/>
-    </row>
-    <row r="42" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D41" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
@@ -1895,7 +1900,9 @@
         <v>35</v>
       </c>
       <c r="C42" s="3"/>
-      <c r="D42" s="2"/>
+      <c r="D42" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="43" spans="1:4" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
@@ -1905,7 +1912,9 @@
         <v>36</v>
       </c>
       <c r="C43" s="3"/>
-      <c r="D43" s="2"/>
+      <c r="D43" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="44" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
@@ -1960,7 +1969,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1974,7 +1983,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2058,7 +2067,7 @@
         <v>16</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2072,7 +2081,7 @@
         <v>16</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2114,7 +2123,7 @@
         <v>16</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2128,10 +2137,10 @@
         <v>16</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -2141,9 +2150,11 @@
       <c r="C60" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D60" s="2"/>
-    </row>
-    <row r="61" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D60" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -2153,9 +2164,11 @@
       <c r="C61" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="2"/>
-    </row>
-    <row r="62" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="D61" s="2" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2169,7 +2182,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
@@ -2183,7 +2196,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>60</v>
       </c>
@@ -2197,7 +2210,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>60</v>
       </c>
@@ -2211,7 +2224,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>60</v>
       </c>
@@ -2225,7 +2238,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>60</v>
       </c>
@@ -2239,7 +2252,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>60</v>
       </c>
@@ -2253,7 +2266,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>60</v>
       </c>
@@ -2267,7 +2280,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>60</v>
       </c>
@@ -2281,18 +2294,18 @@
         <v>266</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>60</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2356,7 +2369,7 @@
         <v>53</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>57</v>
@@ -2365,7 +2378,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
@@ -2375,7 +2388,9 @@
       <c r="C77" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="D77" s="2"/>
+      <c r="D77" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
@@ -2387,7 +2402,9 @@
       <c r="C78" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D78" s="2"/>
+      <c r="D78" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
@@ -2403,7 +2420,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -2413,7 +2430,9 @@
       <c r="C80" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D80" s="2"/>
+      <c r="D80" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
@@ -2425,7 +2444,9 @@
       <c r="C81" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D81" s="2"/>
+      <c r="D81" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
@@ -2452,7 +2473,7 @@
         <v>86</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2465,7 +2486,9 @@
       <c r="C84" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D84" s="2"/>
+      <c r="D84" s="2" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
@@ -3010,7 +3033,7 @@
         <v>261</v>
       </c>
       <c r="D123" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3122,7 +3145,7 @@
         <v>226</v>
       </c>
       <c r="D131" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="132" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3136,7 +3159,7 @@
         <v>226</v>
       </c>
       <c r="D132" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="133" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3237,7 +3260,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>2</v>
       </c>
@@ -3247,9 +3270,11 @@
       <c r="C140" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D140" s="2"/>
-    </row>
-    <row r="141" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D140" s="2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>2</v>
       </c>
@@ -3259,9 +3284,11 @@
       <c r="C141" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D141" s="2"/>
-    </row>
-    <row r="142" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="D141" s="2" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>2</v>
       </c>
@@ -3273,7 +3300,7 @@
       </c>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>2</v>
       </c>
@@ -3295,7 +3322,9 @@
       <c r="C144" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D144" s="2"/>
+      <c r="D144" s="2" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="145" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
@@ -3428,13 +3457,13 @@
         <v>126</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3462,7 +3491,7 @@
         <v>135</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3476,7 +3505,7 @@
         <v>135</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3490,7 +3519,7 @@
         <v>135</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3504,7 +3533,7 @@
         <v>135</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3775,16 +3804,16 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F180" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G180">
         <f>COUNTIF(D:D, "D")</f>
-        <v>144</v>
+        <v>154</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F181" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G181">
         <f>COUNTIF(D:D, "P")</f>
@@ -3793,11 +3822,11 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F182" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G182">
         <f xml:space="preserve"> 178 - G180 -G181</f>
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Jhove dependency and requirements matrix
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="711" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="281">
   <si>
     <t>Requirement</t>
   </si>
@@ -702,9 +702,6 @@
   </si>
   <si>
     <t>The ProjMethodGeoKey SHALL have type = SHORT</t>
-  </si>
-  <si>
-    <t>ProjMethodGeoKey values in the range 1-27 SHALL be GeoTIFF map projection method codes</t>
   </si>
   <si>
     <t>Projection_Definition_GeoKey/ProjMethodGeoKey</t>
@@ -928,6 +925,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Need Help:</t>
+  </si>
+  <si>
+    <t>Not Req:</t>
+  </si>
+  <si>
+    <t>ProjMethodGeoKey values in the range 1-27 SHALL be GeoTIFF map projection method codes (coordinate operation method)</t>
   </si>
 </sst>
 </file>
@@ -1024,7 +1030,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D178">
     <filterColumn colId="3">
-      <filters blank="1"/>
+      <filters>
+        <filter val="P"/>
+      </filters>
     </filterColumn>
   </autoFilter>
   <sortState ref="A2:D187">
@@ -1303,11 +1311,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G182"/>
+  <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F141" sqref="F141"/>
+      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1316,11 +1324,13 @@
     <col min="2" max="2" width="56.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="32.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -1329,7 +1339,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1343,7 +1353,7 @@
         <v>119</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1357,7 +1367,7 @@
         <v>117</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
@@ -1371,7 +1381,7 @@
         <v>125</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1385,7 +1395,7 @@
         <v>121</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1399,7 +1409,7 @@
         <v>123</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1413,7 +1423,7 @@
         <v>183</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1427,7 +1437,7 @@
         <v>183</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1441,7 +1451,7 @@
         <v>183</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -1455,7 +1465,7 @@
         <v>183</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1469,7 +1479,7 @@
         <v>180</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1483,7 +1493,7 @@
         <v>180</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1497,7 +1507,7 @@
         <v>201</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1511,7 +1521,7 @@
         <v>201</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1525,7 +1535,7 @@
         <v>192</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1539,7 +1549,7 @@
         <v>189</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1553,7 +1563,7 @@
         <v>189</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1567,7 +1577,7 @@
         <v>198</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1581,7 +1591,7 @@
         <v>195</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1595,7 +1605,7 @@
         <v>195</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1609,7 +1619,7 @@
         <v>49</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1623,7 +1633,7 @@
         <v>51</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -1637,10 +1647,10 @@
         <v>16</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1651,7 +1661,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1665,7 +1675,7 @@
         <v>16</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1679,7 +1689,7 @@
         <v>102</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1693,7 +1703,7 @@
         <v>102</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1707,7 +1717,7 @@
         <v>102</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1721,7 +1731,7 @@
         <v>102</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -1735,7 +1745,7 @@
         <v>102</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1749,7 +1759,7 @@
         <v>99</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1763,7 +1773,7 @@
         <v>99</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1777,7 +1787,7 @@
         <v>157</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1791,7 +1801,7 @@
         <v>157</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1805,7 +1815,7 @@
         <v>157</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1819,7 +1829,7 @@
         <v>157</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1833,7 +1843,7 @@
         <v>157</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1847,7 +1857,7 @@
         <v>154</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1861,7 +1871,7 @@
         <v>154</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1875,7 +1885,7 @@
         <v>43</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1889,10 +1899,10 @@
         <v>43</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
@@ -1901,7 +1911,7 @@
       </c>
       <c r="C42" s="3"/>
       <c r="D42" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
@@ -1913,7 +1923,7 @@
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1927,7 +1937,7 @@
         <v>32</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1941,7 +1951,7 @@
         <v>32</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1955,10 +1965,10 @@
         <v>13</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
@@ -1969,10 +1979,10 @@
         <v>13</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>14</v>
       </c>
@@ -1983,7 +1993,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1997,7 +2007,7 @@
         <v>13</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2011,7 +2021,7 @@
         <v>13</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2025,7 +2035,7 @@
         <v>13</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -2039,7 +2049,7 @@
         <v>29</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -2053,10 +2063,10 @@
         <v>29</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" ht="32.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
@@ -2067,10 +2077,10 @@
         <v>16</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>14</v>
       </c>
@@ -2081,7 +2091,7 @@
         <v>16</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2095,7 +2105,7 @@
         <v>16</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2109,10 +2119,10 @@
         <v>16</v>
       </c>
       <c r="D57" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>14</v>
       </c>
@@ -2123,10 +2133,10 @@
         <v>16</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>14</v>
       </c>
@@ -2137,10 +2147,10 @@
         <v>16</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -2151,10 +2161,10 @@
         <v>39</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -2165,7 +2175,7 @@
         <v>39</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2179,7 +2189,7 @@
         <v>65</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2193,7 +2203,7 @@
         <v>65</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2207,7 +2217,7 @@
         <v>65</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2221,7 +2231,7 @@
         <v>65</v>
       </c>
       <c r="D65" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2235,7 +2245,7 @@
         <v>65</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2249,7 +2259,7 @@
         <v>65</v>
       </c>
       <c r="D67" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2263,7 +2273,7 @@
         <v>63</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2277,7 +2287,7 @@
         <v>63</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2291,7 +2301,7 @@
         <v>6</v>
       </c>
       <c r="D70" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2299,13 +2309,13 @@
         <v>60</v>
       </c>
       <c r="B71" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>65</v>
       </c>
       <c r="D71" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2319,7 +2329,7 @@
         <v>57</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2333,7 +2343,7 @@
         <v>57</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2347,7 +2357,7 @@
         <v>55</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2361,7 +2371,7 @@
         <v>55</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
@@ -2369,16 +2379,16 @@
         <v>53</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>57</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
@@ -2389,7 +2399,7 @@
         <v>81</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2403,7 +2413,7 @@
         <v>6</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2417,10 +2427,10 @@
         <v>6</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -2431,7 +2441,7 @@
         <v>76</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2445,7 +2455,7 @@
         <v>6</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2459,10 +2469,10 @@
         <v>6</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
@@ -2473,7 +2483,7 @@
         <v>86</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2487,7 +2497,7 @@
         <v>6</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2501,7 +2511,7 @@
         <v>6</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2515,7 +2525,7 @@
         <v>167</v>
       </c>
       <c r="D86" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2529,7 +2539,7 @@
         <v>167</v>
       </c>
       <c r="D87" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2543,7 +2553,7 @@
         <v>167</v>
       </c>
       <c r="D88" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2557,7 +2567,7 @@
         <v>167</v>
       </c>
       <c r="D89" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2571,7 +2581,7 @@
         <v>167</v>
       </c>
       <c r="D90" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2585,7 +2595,7 @@
         <v>164</v>
       </c>
       <c r="D91" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2599,7 +2609,7 @@
         <v>164</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2613,7 +2623,7 @@
         <v>177</v>
       </c>
       <c r="D93" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2627,7 +2637,7 @@
         <v>174</v>
       </c>
       <c r="D94" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2641,203 +2651,203 @@
         <v>174</v>
       </c>
       <c r="D95" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B96" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C96" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C96" s="3" t="s">
-        <v>243</v>
-      </c>
       <c r="D96" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D97" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B98" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D98" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B99" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D99" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B100" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C100" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D100" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B101" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C101" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D101" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B102" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C102" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D102" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B103" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D103" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B104" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="B104" s="3" t="s">
+      <c r="C104" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="C104" s="3" t="s">
-        <v>232</v>
-      </c>
       <c r="D104" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D105" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D106" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B107" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="C107" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="C107" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="D107" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="B108" s="3" t="s">
         <v>244</v>
       </c>
-      <c r="B108" s="3" t="s">
+      <c r="C108" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="C108" s="3" t="s">
-        <v>246</v>
-      </c>
       <c r="D108" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B109" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D109" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -2851,7 +2861,7 @@
         <v>92</v>
       </c>
       <c r="D110" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2865,7 +2875,7 @@
         <v>92</v>
       </c>
       <c r="D111" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2879,7 +2889,7 @@
         <v>92</v>
       </c>
       <c r="D112" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2893,7 +2903,7 @@
         <v>92</v>
       </c>
       <c r="D113" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2907,7 +2917,7 @@
         <v>92</v>
       </c>
       <c r="D114" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2921,7 +2931,7 @@
         <v>89</v>
       </c>
       <c r="D115" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2935,7 +2945,7 @@
         <v>89</v>
       </c>
       <c r="D116" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2949,7 +2959,7 @@
         <v>217</v>
       </c>
       <c r="D117" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2963,7 +2973,7 @@
         <v>217</v>
       </c>
       <c r="D118" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="119" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2977,7 +2987,7 @@
         <v>217</v>
       </c>
       <c r="D119" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="120" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2991,7 +3001,7 @@
         <v>217</v>
       </c>
       <c r="D120" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3005,7 +3015,7 @@
         <v>214</v>
       </c>
       <c r="D121" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="122" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3019,119 +3029,119 @@
         <v>214</v>
       </c>
       <c r="D122" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B123" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="C123" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="C123" s="3" t="s">
-        <v>261</v>
-      </c>
       <c r="D123" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="124" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C124" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D124" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="125" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C125" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D125" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="126" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C126" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D126" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="127" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="B127" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="B127" s="3" t="s">
+      <c r="C127" s="3" t="s">
         <v>251</v>
       </c>
-      <c r="C127" s="3" t="s">
-        <v>252</v>
-      </c>
       <c r="D127" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="128" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B128" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C128" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D128" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="129" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B129" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C129" s="3" t="s">
         <v>254</v>
       </c>
-      <c r="C129" s="3" t="s">
-        <v>255</v>
-      </c>
       <c r="D129" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="130" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B130" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C130" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D130" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="131" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3139,41 +3149,37 @@
         <v>221</v>
       </c>
       <c r="B131" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C131" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D131" s="2" t="s">
-        <v>272</v>
-      </c>
+        <v>225</v>
+      </c>
+      <c r="D131" s="2"/>
     </row>
     <row r="132" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>221</v>
       </c>
       <c r="B132" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="C132" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="C132" s="3" t="s">
-        <v>226</v>
-      </c>
-      <c r="D132" s="2" t="s">
-        <v>271</v>
-      </c>
+      <c r="D132" s="2"/>
     </row>
     <row r="133" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>221</v>
       </c>
       <c r="B133" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D133" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="134" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3181,13 +3187,13 @@
         <v>221</v>
       </c>
       <c r="B134" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C134" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D134" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="135" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3201,7 +3207,7 @@
         <v>223</v>
       </c>
       <c r="D135" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="136" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3215,52 +3221,52 @@
         <v>223</v>
       </c>
       <c r="D136" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="137" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B137" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C137" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D137" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="138" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C138" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D138" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="139" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B139" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="B139" s="3" t="s">
+      <c r="C139" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="C139" s="3" t="s">
-        <v>264</v>
-      </c>
       <c r="D139" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="140" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="140" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>2</v>
       </c>
@@ -3271,10 +3277,10 @@
         <v>13</v>
       </c>
       <c r="D140" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>2</v>
       </c>
@@ -3285,10 +3291,10 @@
         <v>8</v>
       </c>
       <c r="D141" s="2" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="142" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>2</v>
       </c>
@@ -3300,7 +3306,7 @@
       </c>
       <c r="D142" s="2"/>
     </row>
-    <row r="143" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>2</v>
       </c>
@@ -3310,7 +3316,9 @@
       <c r="C143" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D143" s="2"/>
+      <c r="D143" s="2" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="144" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
@@ -3323,7 +3331,7 @@
         <v>6</v>
       </c>
       <c r="D144" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="145" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3337,7 +3345,7 @@
         <v>6</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="146" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3351,7 +3359,7 @@
         <v>128</v>
       </c>
       <c r="D146" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="147" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3365,7 +3373,7 @@
         <v>128</v>
       </c>
       <c r="D147" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="148" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3379,7 +3387,7 @@
         <v>128</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3393,7 +3401,7 @@
         <v>128</v>
       </c>
       <c r="D149" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3407,7 +3415,7 @@
         <v>128</v>
       </c>
       <c r="D150" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3421,7 +3429,7 @@
         <v>128</v>
       </c>
       <c r="D151" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3435,7 +3443,7 @@
         <v>135</v>
       </c>
       <c r="D152" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="153" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3449,21 +3457,21 @@
         <v>135</v>
       </c>
       <c r="D153" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="154" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>126</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="C154" s="3" t="s">
         <v>135</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3477,10 +3485,10 @@
         <v>135</v>
       </c>
       <c r="D155" s="2" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
         <v>126</v>
       </c>
@@ -3491,10 +3499,10 @@
         <v>135</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>126</v>
       </c>
@@ -3505,10 +3513,10 @@
         <v>135</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>126</v>
       </c>
@@ -3519,10 +3527,10 @@
         <v>135</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>126</v>
       </c>
@@ -3533,7 +3541,7 @@
         <v>135</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3547,7 +3555,7 @@
         <v>144</v>
       </c>
       <c r="D160" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="161" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3561,7 +3569,7 @@
         <v>144</v>
       </c>
       <c r="D161" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="162" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3575,7 +3583,7 @@
         <v>144</v>
       </c>
       <c r="D162" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="163" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3589,7 +3597,7 @@
         <v>144</v>
       </c>
       <c r="D163" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="164" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3603,7 +3611,7 @@
         <v>149</v>
       </c>
       <c r="D164" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="165" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3617,7 +3625,7 @@
         <v>149</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -3631,7 +3639,7 @@
         <v>149</v>
       </c>
       <c r="D166" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="167" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3645,7 +3653,7 @@
         <v>205</v>
       </c>
       <c r="D167" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="168" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3659,7 +3667,7 @@
         <v>205</v>
       </c>
       <c r="D168" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="169" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3673,7 +3681,7 @@
         <v>208</v>
       </c>
       <c r="D169" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="170" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3687,7 +3695,7 @@
         <v>208</v>
       </c>
       <c r="D170" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="171" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3701,7 +3709,7 @@
         <v>208</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="172" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3715,7 +3723,7 @@
         <v>208</v>
       </c>
       <c r="D172" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="173" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3729,7 +3737,7 @@
         <v>109</v>
       </c>
       <c r="D173" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="174" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3743,7 +3751,7 @@
         <v>109</v>
       </c>
       <c r="D174" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="175" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3757,7 +3765,7 @@
         <v>112</v>
       </c>
       <c r="D175" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="176" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3765,13 +3773,13 @@
         <v>107</v>
       </c>
       <c r="B176" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="C176" s="3" t="s">
         <v>112</v>
       </c>
       <c r="D176" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="177" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3785,7 +3793,7 @@
         <v>112</v>
       </c>
       <c r="D177" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="178" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3799,12 +3807,12 @@
         <v>112</v>
       </c>
       <c r="D178" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F180" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G180">
         <f>COUNTIF(D:D, "D")</f>
@@ -3813,20 +3821,38 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F181" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G181">
         <f>COUNTIF(D:D, "P")</f>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F182" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G182">
-        <f xml:space="preserve"> 178 - G180 -G181</f>
-        <v>9</v>
+        <f>COUNTIF(D:D, "H")</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F183" t="s">
+        <v>279</v>
+      </c>
+      <c r="G183">
+        <f>COUNTIF(D:D, "N")</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="F184" t="s">
+        <v>274</v>
+      </c>
+      <c r="G184">
+        <f xml:space="preserve"> 177 - G180 - G181 -G182 -G183</f>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Additional EPSG tables and references
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -1028,10 +1028,22 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D178">
-    <filterColumn colId="3">
+  <autoFilter xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" ref="A1:D178">
+    <filterColumn colId="1">
       <filters>
-        <filter val="P"/>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <x14:filter val="If the ProjectionMethodGeoKey value is 32767 (User-Defined) then the ProjectedCitationGeoKey and keys for each map projection parameter (coordinate operation parameter) appropriate to that method SHALL be populated."/>
+            <x14:filter val="ProjectionGeoKey values in the range 1024-32766 SHALL be valid EPSG map projection (coordinate operation) codes"/>
+            <x14:filter val="ProjMethodGeoKey values in the range 1-27 SHALL be GeoTIFF map projection method codes (coordinate operation method)"/>
+            <x14:filter val="The GTModelTypeGeoKey value SHALL be:_x000a_- 0 to indicate that the Model CRS is undefined or unknown_x000a_- 1 to indicate that the Model CRS is a 2D projected Coordinate Reference System, indicated by the value of the ProjectedCRSGeoKey; or_x000a_- 2 to indicate that the Model CRS is a 2DD geographic coordinate reference system, indicated by the value of the GeodeticCRSGeoKey; or_x000a_- 3 to indicate that the Model CRS is a geocentric Cartesian 3D coordinate reference system, indicated by the value of the GeodeticCRSGeoKey; or_x000a_- 32767 to indicate that the Model CRS type is user-defined."/>
+          </mc:Choice>
+          <mc:Fallback>
+            <filter val="If the ProjectionMethodGeoKey value is 32767 (User-Defined) then the ProjectedCitationGeoKey and keys for each map projection parameter (coordinate operation parameter) appropriate to that method SHALL be populated."/>
+            <filter val="ProjectionGeoKey values in the range 1024-32766 SHALL be valid EPSG map projection (coordinate operation) codes"/>
+            <filter val="ProjMethodGeoKey values in the range 1-27 SHALL be GeoTIFF map projection method codes (coordinate operation method)"/>
+          </mc:Fallback>
+        </mc:AlternateContent>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1315,7 +1327,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D55" sqref="D55"/>
+      <selection pane="bottomLeft" activeCell="B71" sqref="B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1650,7 +1662,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1968,7 +1980,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
@@ -1982,7 +1994,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>14</v>
       </c>
@@ -2066,7 +2078,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" ht="32.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
@@ -2080,7 +2092,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>14</v>
       </c>
@@ -2122,7 +2134,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>14</v>
       </c>
@@ -2136,7 +2148,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>14</v>
       </c>
@@ -2304,7 +2316,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>60</v>
       </c>
@@ -2472,7 +2484,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
@@ -2962,7 +2974,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="118" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>212</v>
       </c>
@@ -3032,7 +3044,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>249</v>
       </c>
@@ -3144,7 +3156,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>221</v>
       </c>
@@ -3156,7 +3168,7 @@
       </c>
       <c r="D131" s="2"/>
     </row>
-    <row r="132" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>221</v>
       </c>
@@ -3460,7 +3472,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="154" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>126</v>
       </c>
@@ -3488,7 +3500,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="156" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
         <v>126</v>
       </c>
@@ -3502,7 +3514,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="157" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>126</v>
       </c>
@@ -3516,7 +3528,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="158" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>126</v>
       </c>
@@ -3530,7 +3542,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>126</v>
       </c>

</xml_diff>

<commit_message>
Various clean up and requirement fulfilling
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="281">
   <si>
     <t>Requirement</t>
   </si>
@@ -1029,11 +1029,10 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <autoFilter ref="A1:D178">
-    <filterColumn colId="1">
-      <filters>
-        <filter val="The ModelTiepointTag SHALL have 6 values for each of the K tiepoints"/>
-        <filter val="The ModelTiepointTag SHALL have ID = 33922"/>
-        <filter val="The ModelTiepointTag SHALL have type = DOUBLE"/>
+    <filterColumn colId="3">
+      <filters blank="1">
+        <filter val="H"/>
+        <filter val="P"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -1316,8 +1315,8 @@
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B82" sqref="B82"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D183" sqref="D183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1663,7 +1662,7 @@
         <v>16</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -1981,7 +1980,7 @@
         <v>13</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1995,7 +1994,7 @@
         <v>13</v>
       </c>
       <c r="D48" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2079,7 +2078,7 @@
         <v>16</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
@@ -2093,7 +2092,7 @@
         <v>16</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2135,7 +2134,7 @@
         <v>16</v>
       </c>
       <c r="D58" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2149,10 +2148,10 @@
         <v>16</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -2166,7 +2165,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -2306,7 +2305,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="172.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>60</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -2446,7 +2445,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>72</v>
       </c>
@@ -2460,7 +2459,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>72</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
@@ -3034,7 +3033,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>249</v>
       </c>
@@ -3146,7 +3145,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="131" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>221</v>
       </c>
@@ -3168,7 +3167,9 @@
       <c r="C132" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D132" s="2"/>
+      <c r="D132" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="133" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
@@ -3306,7 +3307,9 @@
       <c r="C142" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D142" s="2"/>
+      <c r="D142" s="2" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="143" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
@@ -3322,7 +3325,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="144" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>2</v>
       </c>
@@ -3473,7 +3476,7 @@
         <v>135</v>
       </c>
       <c r="D154" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3501,7 +3504,7 @@
         <v>135</v>
       </c>
       <c r="D156" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3515,7 +3518,7 @@
         <v>135</v>
       </c>
       <c r="D157" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -3529,7 +3532,7 @@
         <v>135</v>
       </c>
       <c r="D158" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -3543,7 +3546,7 @@
         <v>135</v>
       </c>
       <c r="D159" s="2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
     </row>
     <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -3818,7 +3821,7 @@
       </c>
       <c r="G180">
         <f>COUNTIF(D:D, "D")</f>
-        <v>154</v>
+        <v>168</v>
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.3">
@@ -3827,7 +3830,7 @@
       </c>
       <c r="G181">
         <f>COUNTIF(D:D, "P")</f>
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -3854,7 +3857,7 @@
       </c>
       <c r="G184">
         <f xml:space="preserve"> 177 - G180 - G181 -G182 -G183</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
TODOs and general clean up
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -1315,8 +1315,8 @@
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D183" sqref="D183"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tiff Dump and ASCII fixes
</commit_message>
<xml_diff>
--- a/src/site/Requirements Trace Matrix.xlsx
+++ b/src/site/Requirements Trace Matrix.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="714" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="716" uniqueCount="283">
   <si>
     <t>Requirement</t>
   </si>
@@ -934,6 +934,12 @@
   </si>
   <si>
     <t>ProjMethodGeoKey values in the range 1-27 SHALL be GeoTIFF map projection method codes (coordinate operation method)</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Row-major order cannot be tested.</t>
   </si>
 </sst>
 </file>
@@ -994,7 +1000,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="7">
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1027,23 +1036,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:D178" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D178">
-    <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="H"/>
-        <filter val="P"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState ref="A2:D187">
-    <sortCondition ref="A1:A187"/>
-  </sortState>
-  <tableColumns count="4">
-    <tableColumn id="1" name="Class" dataDxfId="3"/>
-    <tableColumn id="2" name="Requirement" dataDxfId="2"/>
-    <tableColumn id="3" name="Test" dataDxfId="1"/>
-    <tableColumn id="4" name="Status_x000a_(D)one, (P)artial, Need (H)elp, (N)ot Required" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="A1:E178" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <tableColumns count="5">
+    <tableColumn id="1" name="Class" dataDxfId="4"/>
+    <tableColumn id="2" name="Requirement" dataDxfId="3"/>
+    <tableColumn id="3" name="Test" dataDxfId="2"/>
+    <tableColumn id="4" name="Status_x000a_(D)one, (P)artial, Need (H)elp, (N)ot Required" dataDxfId="1"/>
+    <tableColumn id="5" name="Notes" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight16" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1315,8 +1314,8 @@
   <dimension ref="A1:G184"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E85" sqref="E85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1325,11 +1324,12 @@
     <col min="2" max="2" width="56.33203125" customWidth="1"/>
     <col min="3" max="3" width="27.6640625" customWidth="1"/>
     <col min="4" max="4" width="32.5546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
     <col min="6" max="6" width="9.5546875" customWidth="1"/>
     <col min="7" max="7" width="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="24.6" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>266</v>
       </c>
@@ -1342,8 +1342,11 @@
       <c r="D1" s="4" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E1" s="4" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1356,8 +1359,9 @@
       <c r="D2" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>115</v>
       </c>
@@ -1370,8 +1374,9 @@
       <c r="D3" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="129.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>115</v>
       </c>
@@ -1384,8 +1389,9 @@
       <c r="D4" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E4" s="3"/>
+    </row>
+    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>115</v>
       </c>
@@ -1398,8 +1404,9 @@
       <c r="D5" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E5" s="3"/>
+    </row>
+    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>115</v>
       </c>
@@ -1412,8 +1419,9 @@
       <c r="D6" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E6" s="3"/>
+    </row>
+    <row r="7" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>178</v>
       </c>
@@ -1426,8 +1434,9 @@
       <c r="D7" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>178</v>
       </c>
@@ -1440,8 +1449,9 @@
       <c r="D8" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E8" s="3"/>
+    </row>
+    <row r="9" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>178</v>
       </c>
@@ -1454,8 +1464,9 @@
       <c r="D9" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="3"/>
+    </row>
+    <row r="10" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>178</v>
       </c>
@@ -1468,8 +1479,9 @@
       <c r="D10" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E10" s="3"/>
+    </row>
+    <row r="11" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>178</v>
       </c>
@@ -1482,8 +1494,9 @@
       <c r="D11" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>178</v>
       </c>
@@ -1496,8 +1509,9 @@
       <c r="D12" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>199</v>
       </c>
@@ -1510,8 +1524,9 @@
       <c r="D13" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E13" s="3"/>
+    </row>
+    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>199</v>
       </c>
@@ -1524,8 +1539,9 @@
       <c r="D14" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E14" s="3"/>
+    </row>
+    <row r="15" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>187</v>
       </c>
@@ -1538,8 +1554,9 @@
       <c r="D15" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>187</v>
       </c>
@@ -1552,8 +1569,9 @@
       <c r="D16" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="3"/>
+    </row>
+    <row r="17" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>187</v>
       </c>
@@ -1566,8 +1584,9 @@
       <c r="D17" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="3"/>
+    </row>
+    <row r="18" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>193</v>
       </c>
@@ -1580,8 +1599,9 @@
       <c r="D18" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="3"/>
+    </row>
+    <row r="19" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>193</v>
       </c>
@@ -1594,8 +1614,9 @@
       <c r="D19" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E19" s="3"/>
+    </row>
+    <row r="20" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>193</v>
       </c>
@@ -1608,8 +1629,9 @@
       <c r="D20" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E20" s="3"/>
+    </row>
+    <row r="21" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1622,8 +1644,9 @@
       <c r="D21" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" ht="115.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E21" s="3"/>
+    </row>
+    <row r="22" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1636,8 +1659,9 @@
       <c r="D22" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1650,8 +1674,9 @@
       <c r="D23" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E23" s="3"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>45</v>
       </c>
@@ -1664,8 +1689,9 @@
       <c r="D24" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E24" s="3"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>45</v>
       </c>
@@ -1678,8 +1704,9 @@
       <c r="D25" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E25" s="3"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>97</v>
       </c>
@@ -1692,8 +1719,9 @@
       <c r="D26" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E26" s="3"/>
+    </row>
+    <row r="27" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>97</v>
       </c>
@@ -1706,8 +1734,9 @@
       <c r="D27" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="3"/>
+    </row>
+    <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>97</v>
       </c>
@@ -1720,8 +1749,9 @@
       <c r="D28" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E28" s="3"/>
+    </row>
+    <row r="29" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>97</v>
       </c>
@@ -1734,8 +1764,9 @@
       <c r="D29" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E29" s="3"/>
+    </row>
+    <row r="30" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>97</v>
       </c>
@@ -1748,8 +1779,9 @@
       <c r="D30" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="3"/>
+    </row>
+    <row r="31" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>97</v>
       </c>
@@ -1762,8 +1794,9 @@
       <c r="D31" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E31" s="3"/>
+    </row>
+    <row r="32" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>97</v>
       </c>
@@ -1776,8 +1809,9 @@
       <c r="D32" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E32" s="3"/>
+    </row>
+    <row r="33" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>152</v>
       </c>
@@ -1790,8 +1824,9 @@
       <c r="D33" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="3"/>
+    </row>
+    <row r="34" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>152</v>
       </c>
@@ -1804,8 +1839,9 @@
       <c r="D34" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E34" s="3"/>
+    </row>
+    <row r="35" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>152</v>
       </c>
@@ -1818,8 +1854,9 @@
       <c r="D35" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E35" s="3"/>
+    </row>
+    <row r="36" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>152</v>
       </c>
@@ -1832,8 +1869,9 @@
       <c r="D36" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E36" s="3"/>
+    </row>
+    <row r="37" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>152</v>
       </c>
@@ -1846,8 +1884,9 @@
       <c r="D37" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E37" s="3"/>
+    </row>
+    <row r="38" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>152</v>
       </c>
@@ -1860,8 +1899,9 @@
       <c r="D38" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E38" s="3"/>
+    </row>
+    <row r="39" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>152</v>
       </c>
@@ -1874,8 +1914,9 @@
       <c r="D39" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E39" s="3"/>
+    </row>
+    <row r="40" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>41</v>
       </c>
@@ -1888,8 +1929,9 @@
       <c r="D40" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E40" s="3"/>
+    </row>
+    <row r="41" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>41</v>
       </c>
@@ -1902,8 +1944,9 @@
       <c r="D41" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E41" s="3"/>
+    </row>
+    <row r="42" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>34</v>
       </c>
@@ -1914,8 +1957,9 @@
       <c r="D42" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="30" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E42" s="3"/>
+    </row>
+    <row r="43" spans="1:5" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
@@ -1926,8 +1970,9 @@
       <c r="D43" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="3"/>
+    </row>
+    <row r="44" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>14</v>
       </c>
@@ -1940,8 +1985,9 @@
       <c r="D44" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="3"/>
+    </row>
+    <row r="45" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>14</v>
       </c>
@@ -1954,8 +2000,9 @@
       <c r="D45" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="3"/>
+    </row>
+    <row r="46" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>14</v>
       </c>
@@ -1968,8 +2015,9 @@
       <c r="D46" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="3"/>
+    </row>
+    <row r="47" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>14</v>
       </c>
@@ -1982,8 +2030,9 @@
       <c r="D47" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="3"/>
+    </row>
+    <row r="48" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>14</v>
       </c>
@@ -1996,8 +2045,9 @@
       <c r="D48" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="3"/>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>14</v>
       </c>
@@ -2010,8 +2060,9 @@
       <c r="D49" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="3"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>14</v>
       </c>
@@ -2024,8 +2075,9 @@
       <c r="D50" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>14</v>
       </c>
@@ -2038,8 +2090,9 @@
       <c r="D51" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="3"/>
+    </row>
+    <row r="52" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>14</v>
       </c>
@@ -2052,8 +2105,9 @@
       <c r="D52" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E52" s="3"/>
+    </row>
+    <row r="53" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>14</v>
       </c>
@@ -2066,8 +2120,9 @@
       <c r="D53" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" ht="32.4" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E53" s="3"/>
+    </row>
+    <row r="54" spans="1:5" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>14</v>
       </c>
@@ -2080,8 +2135,9 @@
       <c r="D54" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E54" s="3"/>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>14</v>
       </c>
@@ -2094,8 +2150,9 @@
       <c r="D55" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E55" s="3"/>
+    </row>
+    <row r="56" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>14</v>
       </c>
@@ -2108,8 +2165,9 @@
       <c r="D56" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E56" s="3"/>
+    </row>
+    <row r="57" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>14</v>
       </c>
@@ -2122,8 +2180,9 @@
       <c r="D57" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E57" s="3"/>
+    </row>
+    <row r="58" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>14</v>
       </c>
@@ -2136,8 +2195,9 @@
       <c r="D58" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E58" s="3"/>
+    </row>
+    <row r="59" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A59" s="3" t="s">
         <v>14</v>
       </c>
@@ -2150,8 +2210,9 @@
       <c r="D59" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E59" s="3"/>
+    </row>
+    <row r="60" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A60" s="3" t="s">
         <v>37</v>
       </c>
@@ -2164,8 +2225,9 @@
       <c r="D60" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E60" s="3"/>
+    </row>
+    <row r="61" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" s="3" t="s">
         <v>37</v>
       </c>
@@ -2178,8 +2240,9 @@
       <c r="D61" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E61" s="3"/>
+    </row>
+    <row r="62" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A62" s="3" t="s">
         <v>60</v>
       </c>
@@ -2192,8 +2255,9 @@
       <c r="D62" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E62" s="3"/>
+    </row>
+    <row r="63" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
@@ -2206,8 +2270,9 @@
       <c r="D63" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E63" s="3"/>
+    </row>
+    <row r="64" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A64" s="3" t="s">
         <v>60</v>
       </c>
@@ -2220,8 +2285,9 @@
       <c r="D64" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E64" s="3"/>
+    </row>
+    <row r="65" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" s="3" t="s">
         <v>60</v>
       </c>
@@ -2234,8 +2300,9 @@
       <c r="D65" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E65" s="3"/>
+    </row>
+    <row r="66" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
         <v>60</v>
       </c>
@@ -2248,8 +2315,9 @@
       <c r="D66" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E66" s="3"/>
+    </row>
+    <row r="67" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" s="3" t="s">
         <v>60</v>
       </c>
@@ -2262,8 +2330,9 @@
       <c r="D67" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E67" s="3"/>
+    </row>
+    <row r="68" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A68" s="3" t="s">
         <v>60</v>
       </c>
@@ -2276,8 +2345,9 @@
       <c r="D68" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E68" s="3"/>
+    </row>
+    <row r="69" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="3" t="s">
         <v>60</v>
       </c>
@@ -2290,8 +2360,9 @@
       <c r="D69" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E69" s="3"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A70" s="3" t="s">
         <v>60</v>
       </c>
@@ -2304,8 +2375,9 @@
       <c r="D70" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="E70" s="3"/>
+    </row>
+    <row r="71" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A71" s="3" t="s">
         <v>60</v>
       </c>
@@ -2318,8 +2390,9 @@
       <c r="D71" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E71" s="3"/>
+    </row>
+    <row r="72" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A72" s="3" t="s">
         <v>53</v>
       </c>
@@ -2332,8 +2405,9 @@
       <c r="D72" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E72" s="3"/>
+    </row>
+    <row r="73" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" s="3" t="s">
         <v>53</v>
       </c>
@@ -2346,8 +2420,9 @@
       <c r="D73" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E73" s="3"/>
+    </row>
+    <row r="74" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" s="3" t="s">
         <v>53</v>
       </c>
@@ -2360,8 +2435,9 @@
       <c r="D74" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E74" s="3"/>
+    </row>
+    <row r="75" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A75" s="3" t="s">
         <v>53</v>
       </c>
@@ -2374,8 +2450,9 @@
       <c r="D75" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E75" s="3"/>
+    </row>
+    <row r="76" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A76" s="3" t="s">
         <v>53</v>
       </c>
@@ -2388,8 +2465,9 @@
       <c r="D76" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E76" s="3"/>
+    </row>
+    <row r="77" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A77" s="3" t="s">
         <v>77</v>
       </c>
@@ -2402,8 +2480,9 @@
       <c r="D77" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E77" s="3"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="3" t="s">
         <v>77</v>
       </c>
@@ -2416,8 +2495,9 @@
       <c r="D78" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E78" s="3"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A79" s="3" t="s">
         <v>77</v>
       </c>
@@ -2430,8 +2510,9 @@
       <c r="D79" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E79" s="3"/>
+    </row>
+    <row r="80" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A80" s="3" t="s">
         <v>72</v>
       </c>
@@ -2444,8 +2525,9 @@
       <c r="D80" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E80" s="3"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A81" s="3" t="s">
         <v>72</v>
       </c>
@@ -2458,8 +2540,9 @@
       <c r="D81" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="82" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E81" s="3"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A82" s="3" t="s">
         <v>72</v>
       </c>
@@ -2472,8 +2555,9 @@
       <c r="D82" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="83" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="E82" s="3"/>
+    </row>
+    <row r="83" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A83" s="3" t="s">
         <v>82</v>
       </c>
@@ -2484,10 +2568,13 @@
         <v>86</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+      <c r="E83" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A84" s="3" t="s">
         <v>82</v>
       </c>
@@ -2500,8 +2587,9 @@
       <c r="D84" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="85" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E84" s="3"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A85" s="3" t="s">
         <v>82</v>
       </c>
@@ -2514,8 +2602,9 @@
       <c r="D85" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="86" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E85" s="3"/>
+    </row>
+    <row r="86" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A86" s="3" t="s">
         <v>162</v>
       </c>
@@ -2528,8 +2617,9 @@
       <c r="D86" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="87" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E86" s="3"/>
+    </row>
+    <row r="87" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A87" s="3" t="s">
         <v>162</v>
       </c>
@@ -2542,8 +2632,9 @@
       <c r="D87" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="88" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E87" s="3"/>
+    </row>
+    <row r="88" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" s="3" t="s">
         <v>162</v>
       </c>
@@ -2556,8 +2647,9 @@
       <c r="D88" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="89" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E88" s="3"/>
+    </row>
+    <row r="89" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A89" s="3" t="s">
         <v>162</v>
       </c>
@@ -2570,8 +2662,9 @@
       <c r="D89" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="90" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E89" s="3"/>
+    </row>
+    <row r="90" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" s="3" t="s">
         <v>162</v>
       </c>
@@ -2584,8 +2677,9 @@
       <c r="D90" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="91" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E90" s="3"/>
+    </row>
+    <row r="91" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" s="3" t="s">
         <v>162</v>
       </c>
@@ -2598,8 +2692,9 @@
       <c r="D91" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="92" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E91" s="3"/>
+    </row>
+    <row r="92" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" s="3" t="s">
         <v>162</v>
       </c>
@@ -2612,8 +2707,9 @@
       <c r="D92" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="93" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E92" s="3"/>
+    </row>
+    <row r="93" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A93" s="3" t="s">
         <v>172</v>
       </c>
@@ -2626,8 +2722,9 @@
       <c r="D93" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="94" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E93" s="3"/>
+    </row>
+    <row r="94" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A94" s="3" t="s">
         <v>172</v>
       </c>
@@ -2640,8 +2737,9 @@
       <c r="D94" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="95" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E94" s="3"/>
+    </row>
+    <row r="95" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A95" s="3" t="s">
         <v>172</v>
       </c>
@@ -2654,8 +2752,9 @@
       <c r="D95" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="96" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E95" s="3"/>
+    </row>
+    <row r="96" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A96" s="3" t="s">
         <v>229</v>
       </c>
@@ -2668,8 +2767,9 @@
       <c r="D96" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="97" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E96" s="3"/>
+    </row>
+    <row r="97" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A97" s="3" t="s">
         <v>229</v>
       </c>
@@ -2682,8 +2782,9 @@
       <c r="D97" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="98" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E97" s="3"/>
+    </row>
+    <row r="98" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A98" s="3" t="s">
         <v>229</v>
       </c>
@@ -2696,8 +2797,9 @@
       <c r="D98" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="99" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E98" s="3"/>
+    </row>
+    <row r="99" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" s="3" t="s">
         <v>229</v>
       </c>
@@ -2710,8 +2812,9 @@
       <c r="D99" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="100" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E99" s="3"/>
+    </row>
+    <row r="100" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
         <v>229</v>
       </c>
@@ -2724,8 +2827,9 @@
       <c r="D100" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="101" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" s="3" t="s">
         <v>229</v>
       </c>
@@ -2738,8 +2842,9 @@
       <c r="D101" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="102" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E101" s="3"/>
+    </row>
+    <row r="102" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="3" t="s">
         <v>229</v>
       </c>
@@ -2752,8 +2857,9 @@
       <c r="D102" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="103" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E102" s="3"/>
+    </row>
+    <row r="103" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A103" s="3" t="s">
         <v>229</v>
       </c>
@@ -2766,8 +2872,9 @@
       <c r="D103" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="104" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E103" s="3"/>
+    </row>
+    <row r="104" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A104" s="3" t="s">
         <v>229</v>
       </c>
@@ -2780,8 +2887,9 @@
       <c r="D104" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="105" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E104" s="3"/>
+    </row>
+    <row r="105" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A105" s="3" t="s">
         <v>229</v>
       </c>
@@ -2794,8 +2902,9 @@
       <c r="D105" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="106" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E105" s="3"/>
+    </row>
+    <row r="106" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A106" s="3" t="s">
         <v>229</v>
       </c>
@@ -2808,8 +2917,9 @@
       <c r="D106" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="107" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E106" s="3"/>
+    </row>
+    <row r="107" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" s="3" t="s">
         <v>243</v>
       </c>
@@ -2822,8 +2932,9 @@
       <c r="D107" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="108" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E107" s="3"/>
+    </row>
+    <row r="108" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="3" t="s">
         <v>243</v>
       </c>
@@ -2836,8 +2947,9 @@
       <c r="D108" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="109" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E108" s="3"/>
+    </row>
+    <row r="109" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" s="3" t="s">
         <v>243</v>
       </c>
@@ -2850,8 +2962,9 @@
       <c r="D109" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="110" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E109" s="3"/>
+    </row>
+    <row r="110" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A110" s="3" t="s">
         <v>87</v>
       </c>
@@ -2864,8 +2977,9 @@
       <c r="D110" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="111" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E110" s="3"/>
+    </row>
+    <row r="111" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A111" s="3" t="s">
         <v>87</v>
       </c>
@@ -2878,8 +2992,9 @@
       <c r="D111" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="112" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E111" s="3"/>
+    </row>
+    <row r="112" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A112" s="3" t="s">
         <v>87</v>
       </c>
@@ -2892,8 +3007,9 @@
       <c r="D112" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="113" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E112" s="3"/>
+    </row>
+    <row r="113" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="3" t="s">
         <v>87</v>
       </c>
@@ -2906,8 +3022,9 @@
       <c r="D113" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="114" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E113" s="3"/>
+    </row>
+    <row r="114" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" s="3" t="s">
         <v>87</v>
       </c>
@@ -2920,8 +3037,9 @@
       <c r="D114" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="115" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E114" s="3"/>
+    </row>
+    <row r="115" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A115" s="3" t="s">
         <v>87</v>
       </c>
@@ -2934,8 +3052,9 @@
       <c r="D115" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="116" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E115" s="3"/>
+    </row>
+    <row r="116" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A116" s="3" t="s">
         <v>87</v>
       </c>
@@ -2948,8 +3067,9 @@
       <c r="D116" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="117" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E116" s="3"/>
+    </row>
+    <row r="117" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
         <v>212</v>
       </c>
@@ -2962,8 +3082,9 @@
       <c r="D117" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="118" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E117" s="3"/>
+    </row>
+    <row r="118" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A118" s="3" t="s">
         <v>212</v>
       </c>
@@ -2976,8 +3097,9 @@
       <c r="D118" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="119" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E118" s="3"/>
+    </row>
+    <row r="119" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" s="3" t="s">
         <v>212</v>
       </c>
@@ -2990,8 +3112,9 @@
       <c r="D119" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="120" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E119" s="3"/>
+    </row>
+    <row r="120" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
         <v>212</v>
       </c>
@@ -3004,8 +3127,9 @@
       <c r="D120" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="121" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E120" s="3"/>
+    </row>
+    <row r="121" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A121" s="3" t="s">
         <v>212</v>
       </c>
@@ -3018,8 +3142,9 @@
       <c r="D121" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="122" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E121" s="3"/>
+    </row>
+    <row r="122" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" s="3" t="s">
         <v>212</v>
       </c>
@@ -3032,8 +3157,9 @@
       <c r="D122" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="123" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E122" s="3"/>
+    </row>
+    <row r="123" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="3" t="s">
         <v>249</v>
       </c>
@@ -3046,8 +3172,9 @@
       <c r="D123" s="2" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="124" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E123" s="3"/>
+    </row>
+    <row r="124" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
         <v>249</v>
       </c>
@@ -3060,8 +3187,9 @@
       <c r="D124" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="125" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E124" s="3"/>
+    </row>
+    <row r="125" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A125" s="3" t="s">
         <v>249</v>
       </c>
@@ -3074,8 +3202,9 @@
       <c r="D125" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="126" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E125" s="3"/>
+    </row>
+    <row r="126" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A126" s="3" t="s">
         <v>249</v>
       </c>
@@ -3088,8 +3217,9 @@
       <c r="D126" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="127" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E126" s="3"/>
+    </row>
+    <row r="127" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A127" s="3" t="s">
         <v>249</v>
       </c>
@@ -3102,8 +3232,9 @@
       <c r="D127" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="128" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E127" s="3"/>
+    </row>
+    <row r="128" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A128" s="3" t="s">
         <v>249</v>
       </c>
@@ -3116,8 +3247,9 @@
       <c r="D128" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E128" s="3"/>
+    </row>
+    <row r="129" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A129" s="3" t="s">
         <v>249</v>
       </c>
@@ -3130,8 +3262,9 @@
       <c r="D129" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" ht="72" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E129" s="3"/>
+    </row>
+    <row r="130" spans="1:5" ht="72" x14ac:dyDescent="0.3">
       <c r="A130" s="3" t="s">
         <v>249</v>
       </c>
@@ -3144,8 +3277,9 @@
       <c r="D130" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="E130" s="3"/>
+    </row>
+    <row r="131" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A131" s="3" t="s">
         <v>221</v>
       </c>
@@ -3156,8 +3290,9 @@
         <v>225</v>
       </c>
       <c r="D131" s="2"/>
-    </row>
-    <row r="132" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E131" s="3"/>
+    </row>
+    <row r="132" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A132" s="3" t="s">
         <v>221</v>
       </c>
@@ -3170,8 +3305,9 @@
       <c r="D132" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E132" s="3"/>
+    </row>
+    <row r="133" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A133" s="3" t="s">
         <v>221</v>
       </c>
@@ -3184,8 +3320,9 @@
       <c r="D133" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E133" s="3"/>
+    </row>
+    <row r="134" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A134" s="3" t="s">
         <v>221</v>
       </c>
@@ -3198,8 +3335,9 @@
       <c r="D134" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E134" s="3"/>
+    </row>
+    <row r="135" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A135" s="3" t="s">
         <v>221</v>
       </c>
@@ -3212,8 +3350,9 @@
       <c r="D135" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="136" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E135" s="3"/>
+    </row>
+    <row r="136" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A136" s="3" t="s">
         <v>221</v>
       </c>
@@ -3226,8 +3365,9 @@
       <c r="D136" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="137" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E136" s="3"/>
+    </row>
+    <row r="137" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A137" s="3" t="s">
         <v>261</v>
       </c>
@@ -3240,8 +3380,9 @@
       <c r="D137" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="138" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E137" s="3"/>
+    </row>
+    <row r="138" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A138" s="3" t="s">
         <v>261</v>
       </c>
@@ -3254,8 +3395,9 @@
       <c r="D138" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="139" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E138" s="3"/>
+    </row>
+    <row r="139" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A139" s="3" t="s">
         <v>261</v>
       </c>
@@ -3268,8 +3410,9 @@
       <c r="D139" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="140" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E139" s="3"/>
+    </row>
+    <row r="140" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
         <v>2</v>
       </c>
@@ -3282,8 +3425,9 @@
       <c r="D140" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="141" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E140" s="3"/>
+    </row>
+    <row r="141" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A141" s="3" t="s">
         <v>2</v>
       </c>
@@ -3296,8 +3440,9 @@
       <c r="D141" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E141" s="3"/>
+    </row>
+    <row r="142" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A142" s="3" t="s">
         <v>2</v>
       </c>
@@ -3310,8 +3455,9 @@
       <c r="D142" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E142" s="3"/>
+    </row>
+    <row r="143" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A143" s="3" t="s">
         <v>2</v>
       </c>
@@ -3324,8 +3470,9 @@
       <c r="D143" s="2" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="144" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="E143" s="3"/>
+    </row>
+    <row r="144" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A144" s="3" t="s">
         <v>2</v>
       </c>
@@ -3338,8 +3485,9 @@
       <c r="D144" s="2" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="145" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E144" s="3"/>
+    </row>
+    <row r="145" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A145" s="3" t="s">
         <v>2</v>
       </c>
@@ -3352,8 +3500,9 @@
       <c r="D145" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="146" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E145" s="3"/>
+    </row>
+    <row r="146" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A146" s="3" t="s">
         <v>126</v>
       </c>
@@ -3366,8 +3515,9 @@
       <c r="D146" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="147" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E146" s="3"/>
+    </row>
+    <row r="147" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A147" s="3" t="s">
         <v>126</v>
       </c>
@@ -3380,8 +3530,9 @@
       <c r="D147" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="148" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E147" s="3"/>
+    </row>
+    <row r="148" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="3" t="s">
         <v>126</v>
       </c>
@@ -3394,8 +3545,9 @@
       <c r="D148" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="149" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E148" s="3"/>
+    </row>
+    <row r="149" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A149" s="3" t="s">
         <v>126</v>
       </c>
@@ -3408,8 +3560,9 @@
       <c r="D149" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="150" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E149" s="3"/>
+    </row>
+    <row r="150" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A150" s="3" t="s">
         <v>126</v>
       </c>
@@ -3422,8 +3575,9 @@
       <c r="D150" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="151" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E150" s="3"/>
+    </row>
+    <row r="151" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A151" s="3" t="s">
         <v>126</v>
       </c>
@@ -3436,8 +3590,9 @@
       <c r="D151" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="152" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E151" s="3"/>
+    </row>
+    <row r="152" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A152" s="3" t="s">
         <v>126</v>
       </c>
@@ -3450,8 +3605,9 @@
       <c r="D152" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="153" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E152" s="3"/>
+    </row>
+    <row r="153" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A153" s="3" t="s">
         <v>126</v>
       </c>
@@ -3464,8 +3620,9 @@
       <c r="D153" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="154" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E153" s="3"/>
+    </row>
+    <row r="154" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A154" s="3" t="s">
         <v>126</v>
       </c>
@@ -3478,8 +3635,9 @@
       <c r="D154" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="155" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E154" s="3"/>
+    </row>
+    <row r="155" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A155" s="3" t="s">
         <v>126</v>
       </c>
@@ -3492,8 +3650,9 @@
       <c r="D155" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="156" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E155" s="3"/>
+    </row>
+    <row r="156" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A156" s="3" t="s">
         <v>126</v>
       </c>
@@ -3506,8 +3665,9 @@
       <c r="D156" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="157" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E156" s="3"/>
+    </row>
+    <row r="157" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A157" s="3" t="s">
         <v>126</v>
       </c>
@@ -3520,8 +3680,9 @@
       <c r="D157" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="158" spans="1:4" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E157" s="3"/>
+    </row>
+    <row r="158" spans="1:5" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A158" s="3" t="s">
         <v>126</v>
       </c>
@@ -3534,8 +3695,9 @@
       <c r="D158" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="159" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E158" s="3"/>
+    </row>
+    <row r="159" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A159" s="3" t="s">
         <v>126</v>
       </c>
@@ -3548,8 +3710,9 @@
       <c r="D159" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="160" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E159" s="3"/>
+    </row>
+    <row r="160" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A160" s="3" t="s">
         <v>142</v>
       </c>
@@ -3562,8 +3725,9 @@
       <c r="D160" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="161" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E160" s="3"/>
+    </row>
+    <row r="161" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
         <v>142</v>
       </c>
@@ -3576,8 +3740,9 @@
       <c r="D161" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="162" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E161" s="3"/>
+    </row>
+    <row r="162" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A162" s="3" t="s">
         <v>142</v>
       </c>
@@ -3590,8 +3755,9 @@
       <c r="D162" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="163" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E162" s="3"/>
+    </row>
+    <row r="163" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A163" s="3" t="s">
         <v>142</v>
       </c>
@@ -3604,8 +3770,9 @@
       <c r="D163" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="164" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E163" s="3"/>
+    </row>
+    <row r="164" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A164" s="3" t="s">
         <v>142</v>
       </c>
@@ -3618,8 +3785,9 @@
       <c r="D164" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="165" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E164" s="3"/>
+    </row>
+    <row r="165" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A165" s="3" t="s">
         <v>142</v>
       </c>
@@ -3632,8 +3800,9 @@
       <c r="D165" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="166" spans="1:4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E165" s="3"/>
+    </row>
+    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" s="3" t="s">
         <v>142</v>
       </c>
@@ -3646,8 +3815,9 @@
       <c r="D166" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="167" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E166" s="3"/>
+    </row>
+    <row r="167" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A167" s="3" t="s">
         <v>203</v>
       </c>
@@ -3660,8 +3830,9 @@
       <c r="D167" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="168" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E167" s="3"/>
+    </row>
+    <row r="168" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A168" s="3" t="s">
         <v>203</v>
       </c>
@@ -3674,8 +3845,9 @@
       <c r="D168" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="169" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E168" s="3"/>
+    </row>
+    <row r="169" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A169" s="3" t="s">
         <v>203</v>
       </c>
@@ -3688,8 +3860,9 @@
       <c r="D169" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="170" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E169" s="3"/>
+    </row>
+    <row r="170" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A170" s="3" t="s">
         <v>203</v>
       </c>
@@ -3702,8 +3875,9 @@
       <c r="D170" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="171" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E170" s="3"/>
+    </row>
+    <row r="171" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A171" s="3" t="s">
         <v>203</v>
       </c>
@@ -3716,8 +3890,9 @@
       <c r="D171" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="172" spans="1:4" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E171" s="3"/>
+    </row>
+    <row r="172" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
         <v>203</v>
       </c>
@@ -3730,8 +3905,9 @@
       <c r="D172" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="173" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E172" s="3"/>
+    </row>
+    <row r="173" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A173" s="3" t="s">
         <v>107</v>
       </c>
@@ -3744,8 +3920,9 @@
       <c r="D173" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="174" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E173" s="3"/>
+    </row>
+    <row r="174" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A174" s="3" t="s">
         <v>107</v>
       </c>
@@ -3758,8 +3935,9 @@
       <c r="D174" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="175" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E174" s="3"/>
+    </row>
+    <row r="175" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A175" s="3" t="s">
         <v>107</v>
       </c>
@@ -3772,8 +3950,9 @@
       <c r="D175" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="176" spans="1:4" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E175" s="3"/>
+    </row>
+    <row r="176" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A176" s="3" t="s">
         <v>107</v>
       </c>
@@ -3786,8 +3965,9 @@
       <c r="D176" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="177" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E176" s="3"/>
+    </row>
+    <row r="177" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A177" s="3" t="s">
         <v>107</v>
       </c>
@@ -3800,8 +3980,9 @@
       <c r="D177" s="2" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="178" spans="1:7" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="E177" s="3"/>
+    </row>
+    <row r="178" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A178" s="3" t="s">
         <v>107</v>
       </c>
@@ -3814,6 +3995,7 @@
       <c r="D178" s="2" t="s">
         <v>265</v>
       </c>
+      <c r="E178" s="3"/>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.3">
       <c r="F180" t="s">
@@ -3830,7 +4012,7 @@
       </c>
       <c r="G181">
         <f>COUNTIF(D:D, "P")</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.3">
@@ -3848,7 +4030,7 @@
       </c>
       <c r="G183">
         <f>COUNTIF(D:D, "N")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>